<commit_message>
update the flood report
</commit_message>
<xml_diff>
--- a/automatic docx/database_report.xlsx
+++ b/automatic docx/database_report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Python Scripts\automatic docx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39DA225-20FC-49B3-8642-46529BE56A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667CFB5F-30E3-417B-BC54-9C944185E443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{83108E16-E9D6-4CCB-B5BE-A67101359CD3}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="398">
   <si>
     <t>fecha_emision</t>
   </si>
@@ -1171,9 +1171,6 @@
     <t>Frase completa</t>
   </si>
   <si>
-    <t xml:space="preserve">En las últimas horas se registraron importantes acumulados de precipitación en la cuenca del río Yí, donde en las últimas 72 horas se acumularon 125.4 mm y con un máximo de 100 mm/día. Actualmente, el nivel del río Yí está en ascenso en la ciudad de Durazno.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  Existe una alta probabilidad de que el nivel supere al máximo registrado los días anteriores (2.3 metros). </t>
-  </si>
-  <si>
     <t>En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Santa Lucía, donde en las últimas 72 horas se acumularon 105 mm y con un máximo de 35 mm/día. Actualmente, el nivel del río Santa Lucía está en ascenso en la ciudad de Santa Lucía.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  Existe una baja probabilidad de que el nivel supere al máximo registrado los días anteriores (8 metros), pero no se puede descartar en su totalidad.</t>
   </si>
   <si>
@@ -1198,28 +1195,46 @@
     <t>En las últimas horas se registraron bajos acumulados de precipitación en la cuenca del río Uruguay, donde en las últimas 72 horas se acumularon 0 mm y con un máximo de 0 mm/día. Actualmente, el nivel del río Uruguay está en ascenso en las ciudades de Bella Unión Paysandú; se mantiene constante en las ciudades de Salto Fray Bentos. está en descenso en la ciudad de . Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  Existe una alta probabilidad de que el nivel supere al máximo registrado los días anteriores (5m en Paysandú ).</t>
   </si>
   <si>
-    <t>Entre 10.00 y 10.60</t>
-  </si>
-  <si>
-    <t>02 - 03 dic</t>
-  </si>
-  <si>
-    <t>Entre 9.46 y 10.22</t>
-  </si>
-  <si>
-    <t>03 - 05 dic</t>
-  </si>
-  <si>
-    <t>Entre 9.00 y 10.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Cuareim, donde en las últimas 24 horas se acumularon 70 mm. Actualmente, el nivel del río Cuareim está en ascenso en la ciudad de Artigas.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, se espera que el nivel del río Cuareim en Artigas supere la cota de aviso (8.00 m) generando inundaciones en la zona del paseo 7 de setiembre. Dado que el nivel pronosticado esta cerca de la cota de seguridad (10.20 m) no se descarta completamenta esta posibilidad. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Estar atentos a posibles inundaciones locales en la zona del paseo 7 de setiembre. </t>
   </si>
   <si>
-    <t>Se registra incrementos del río Cuareim en Artigas con posibilidad de afectar zona paseo 7 de setiembre</t>
+    <t>Se registra incrementos del río Cuareim en Artigas con baja posibilidad de afectar la zona del paseo 7 de setiembre</t>
+  </si>
+  <si>
+    <t>Menor a 2.0 m</t>
+  </si>
+  <si>
+    <t>17 - 18 Enero</t>
+  </si>
+  <si>
+    <t>18 - 20 Enero</t>
+  </si>
+  <si>
+    <t>Menor a 5.0 m</t>
+  </si>
+  <si>
+    <t>Menor a 3.5 m</t>
+  </si>
+  <si>
+    <t>19 - 21 Enero</t>
+  </si>
+  <si>
+    <t>Menor a 5.9 m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Yí, donde en las últimas 24 horas se acumularon 45.7 mm. Actualmente, el nivel del río Yí se mantiene constante en la ciudad de Durazno.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días, con una baja probabilidad de generarse afectaciones a vivienda en la ciudad de Durazno. </t>
+  </si>
+  <si>
+    <t>Entre 8.20 a 8.50 m</t>
+  </si>
+  <si>
+    <t>Entre 6.30 a 6.70 m</t>
+  </si>
+  <si>
+    <t>18 - 19 Enero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Cuareim, donde en las últimas 24 horas se acumularon 55.5 mm. Actualmente, el nivel del río Cuareim está en ascenso en la ciudad de Artigas.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días, el cual se estima que llegue a un nivel entre 6.30 a 6.70 metros y con una bjaa probabilidad de generarse inundaciones en la zona del paseo 7 de setiembre  </t>
   </si>
 </sst>
 </file>
@@ -1751,9 +1766,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1791,7 +1806,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1897,7 +1912,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2039,7 +2054,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2082,7 +2097,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="41">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2094,7 +2109,7 @@
       </c>
       <c r="C3" s="42">
         <f ca="1">TODAY()</f>
-        <v>45262</v>
+        <v>45308</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -2106,7 +2121,7 @@
       </c>
       <c r="C4" s="43">
         <f ca="1">$C$3-1</f>
-        <v>45261</v>
+        <v>45307</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2118,7 +2133,7 @@
       </c>
       <c r="C5" s="42">
         <f ca="1">$C$3-2</f>
-        <v>45260</v>
+        <v>45306</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -2130,7 +2145,7 @@
       </c>
       <c r="C6" s="43">
         <f ca="1">$C$3+1</f>
-        <v>45263</v>
+        <v>45309</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -2142,7 +2157,7 @@
       </c>
       <c r="C7" s="44">
         <f ca="1">$C$3+2</f>
-        <v>45264</v>
+        <v>45310</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2154,7 +2169,7 @@
       </c>
       <c r="C8" s="42">
         <f ca="1">$C$3+3</f>
-        <v>45265</v>
+        <v>45311</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2165,7 +2180,7 @@
         <v>174</v>
       </c>
       <c r="C9" s="45" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -2179,8 +2194,8 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2210,7 +2225,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="8">
-        <v>6.1</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2221,7 +2236,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="6">
-        <v>6.9</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2233,7 +2248,7 @@
       </c>
       <c r="C4" s="32">
         <f>IFERROR(ROUND(ABS(C2-C3)*100,0),"-")</f>
-        <v>80</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2245,7 +2260,7 @@
       </c>
       <c r="C5" s="39" t="str">
         <f>IFERROR(IF(C4=0,"Permanece",IF(SIGN(C4)=1,"Sube","Baja")),"-")</f>
-        <v>Sube</v>
+        <v>Permanece</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2256,7 +2271,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="8">
-        <v>5.4</v>
+        <v>2.0499999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2267,7 +2282,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="6">
-        <v>5.2</v>
+        <v>2.0499999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2290,7 +2305,7 @@
       </c>
       <c r="C9" s="32">
         <f>IF((C6-C7)&gt;=0,ROUND((C6-C7)*100,0),"")</f>
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2302,7 +2317,7 @@
       </c>
       <c r="C10" s="39" t="str">
         <f>IF(C9=0,"Permanece",IF(C9="","Baja","Sube"))</f>
-        <v>Sube</v>
+        <v>Permanece</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2313,7 +2328,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="8">
-        <v>2.1</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2324,7 +2339,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="6">
-        <v>1.9</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2347,7 +2362,7 @@
       </c>
       <c r="C14" s="32">
         <f>IF((C11-C12)&gt;=0,ROUND((C11-C12)*100,0),"")</f>
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2359,7 +2374,7 @@
       </c>
       <c r="C15" s="39" t="str">
         <f>IF(C14=0,"Permanece",IF(C14="","Baja","Sube"))</f>
-        <v>Sube</v>
+        <v>Permanece</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2369,9 +2384,7 @@
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="6">
-        <v>2.6</v>
-      </c>
+      <c r="C16" s="6"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
@@ -2380,9 +2393,7 @@
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="6">
-        <v>2.4</v>
-      </c>
+      <c r="C17" s="6"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
@@ -2404,7 +2415,7 @@
       </c>
       <c r="C19" s="32">
         <f>IF((C16-C17)&gt;=0,ROUND((C16-C17)*100,0),"")</f>
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2416,7 +2427,7 @@
       </c>
       <c r="C20" s="39" t="str">
         <f>IF(C19=0,"Permanece",IF(C19="","Baja","Sube"))</f>
-        <v>Sube</v>
+        <v>Permanece</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2427,7 +2438,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="8">
-        <v>20.399999999999999</v>
+        <v>45.7</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2438,7 +2449,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="6">
-        <v>100</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2449,7 +2460,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="6">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2460,7 +2471,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="6">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2471,7 +2482,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="6">
-        <v>80</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2482,7 +2493,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="10">
-        <v>65</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2492,8 +2503,8 @@
       <c r="B27" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="11">
-        <v>7.2</v>
+      <c r="C27" s="11" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2504,7 +2515,7 @@
         <v>36</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>40</v>
+        <v>387</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2514,8 +2525,8 @@
       <c r="B29" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="11">
-        <v>8.9</v>
+      <c r="C29" s="11" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2526,7 +2537,7 @@
         <v>37</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>40</v>
+        <v>388</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2536,8 +2547,8 @@
       <c r="B31" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="11">
-        <v>2.5</v>
+      <c r="C31" s="11" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2548,7 +2559,7 @@
         <v>38</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>40</v>
+        <v>391</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2559,7 +2570,7 @@
         <v>29</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>35</v>
+        <v>392</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2570,7 +2581,7 @@
         <v>39</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>40</v>
+        <v>391</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="198.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2581,7 +2592,7 @@
         <v>41</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>376</v>
+        <v>393</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2623,7 +2634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D9A6E30-A876-45F0-8067-30FAF0E80436}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -2654,7 +2665,7 @@
         <v>85</v>
       </c>
       <c r="C2" s="6">
-        <v>5.95</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2665,7 +2676,7 @@
         <v>86</v>
       </c>
       <c r="C3" s="6">
-        <v>5.59</v>
+        <v>5.75</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2686,9 +2697,9 @@
       <c r="B5" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="32" t="str">
         <f>IF((C2-C3)&gt;=0,ROUND((C2-C3)*100,0),"")</f>
-        <v>36</v>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2700,7 +2711,7 @@
       </c>
       <c r="C6" s="39" t="str">
         <f>IF(C5=0,"Permanece",IF(C5="","Baja","Sube"))</f>
-        <v>Sube</v>
+        <v>Baja</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2711,7 +2722,7 @@
         <v>91</v>
       </c>
       <c r="C7" s="6">
-        <v>4</v>
+        <v>7.59</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2722,7 +2733,7 @@
         <v>92</v>
       </c>
       <c r="C8" s="6">
-        <v>3.68</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2745,7 +2756,7 @@
       </c>
       <c r="C10" s="32">
         <f>IF((C7-C8)&gt;=0,ROUND((C7-C8)*100,0),"")</f>
-        <v>32</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2768,7 +2779,7 @@
         <v>97</v>
       </c>
       <c r="C12" s="6">
-        <v>4.16</v>
+        <v>5.16</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2779,7 +2790,7 @@
         <v>98</v>
       </c>
       <c r="C13" s="6">
-        <v>3.69</v>
+        <v>4.88</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2802,7 +2813,7 @@
       </c>
       <c r="C15" s="32">
         <f>IF((C12-C13)&gt;=0,ROUND((C12-C13)*100,0),"")</f>
-        <v>47</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2825,7 +2836,7 @@
         <v>77</v>
       </c>
       <c r="C17" s="8">
-        <v>70</v>
+        <v>55.5</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -2858,7 +2869,7 @@
         <v>80</v>
       </c>
       <c r="C20" s="6">
-        <v>59.5</v>
+        <v>13.9</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -2869,7 +2880,7 @@
         <v>81</v>
       </c>
       <c r="C21" s="6">
-        <v>26.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2880,7 +2891,7 @@
         <v>82</v>
       </c>
       <c r="C22" s="10">
-        <v>0.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -2890,9 +2901,7 @@
       <c r="B23" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C23" s="11" t="s">
-        <v>385</v>
-      </c>
+      <c r="C23" s="11"/>
     </row>
     <row r="24" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="29" t="s">
@@ -2901,9 +2910,7 @@
       <c r="B24" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>386</v>
-      </c>
+      <c r="C24" s="12"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="28" t="s">
@@ -2913,7 +2920,7 @@
         <v>95</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>387</v>
+        <v>394</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2924,7 +2931,7 @@
         <v>96</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -2935,7 +2942,7 @@
         <v>101</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2946,10 +2953,10 @@
         <v>102</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="231.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="215.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="28" t="s">
         <v>67</v>
       </c>
@@ -2957,7 +2964,7 @@
         <v>83</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>390</v>
+        <v>397</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2968,7 +2975,7 @@
         <v>84</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -3529,7 +3536,7 @@
         <v>121</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3924,7 +3931,7 @@
         <v>180</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3935,7 +3942,7 @@
         <v>175</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3946,7 +3953,7 @@
         <v>176</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -3957,7 +3964,7 @@
         <v>203</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3968,7 +3975,7 @@
         <v>204</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -3979,7 +3986,7 @@
         <v>205</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3990,7 +3997,7 @@
         <v>206</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -4012,7 +4019,7 @@
         <v>210</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="248.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4023,7 +4030,7 @@
         <v>202</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4308,7 +4315,7 @@
         <v>255</v>
       </c>
       <c r="C21" s="72" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4638,13 +4645,13 @@
       </c>
       <c r="F23" s="54" t="str">
         <f>_xlfn.CONCAT(IF(OR(MAX(YI!C21:C23)&gt;$D$3,SUM(YI!C21:C23)&gt;$E$3),$F$3,IF(OR(MAX(YI!C21:C23)&gt;$D$4,SUM(YI!C21:C23)&gt;$E$4),$F$4,$F$5)),D23,$I$3,SUM(YI!C21:C23),$J$3,MAX(YI!C21:C23),$K$3)</f>
-        <v>En las últimas horas se registraron importantes acumulados de precipitación en la cuenca del río Yí, donde en las últimas 72 horas se acumularon 125.4 mm y con un máximo de 100 mm/día.</v>
+        <v>En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Yí, donde en las últimas 72 horas se acumularon 47.7 mm y con un máximo de 45.7 mm/día.</v>
       </c>
       <c r="G23" s="54"/>
       <c r="H23" s="54"/>
       <c r="I23" s="54" t="str">
         <f>_xlfn.CONCAT($F$8,D23,IF(YI!C15=$E$8,$I$8,IF(YI!C15=$E$9,$I$9,$I$10)),$J$8,E23,". ")</f>
-        <v xml:space="preserve">Actualmente, el nivel del río Yí está en ascenso en la ciudad de Durazno. </v>
+        <v xml:space="preserve">Actualmente, el nivel del río Yí se mantiene constante en la ciudad de Durazno. </v>
       </c>
       <c r="J23" s="54" t="str">
         <f>_xlfn.CONCAT(F13,IF(YI!C31&gt;YI!C11,I13, IF(YI!C31=YI!C11,I14, I15)))</f>
@@ -4656,7 +4663,7 @@
       </c>
       <c r="L23" s="54" t="str">
         <f>+_xlfn.CONCAT(F23," ",I23, " ",J23," ",K23)</f>
-        <v xml:space="preserve">En las últimas horas se registraron importantes acumulados de precipitación en la cuenca del río Yí, donde en las últimas 72 horas se acumularon 125.4 mm y con un máximo de 100 mm/día. Actualmente, el nivel del río Yí está en ascenso en la ciudad de Durazno.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  Existe una alta probabilidad de que el nivel supere al máximo registrado los días anteriores (2.3 metros). </v>
+        <v xml:space="preserve">En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Yí, donde en las últimas 72 horas se acumularon 47.7 mm y con un máximo de 45.7 mm/día. Actualmente, el nivel del río Yí se mantiene constante en la ciudad de Durazno.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  Existe una alta probabilidad de que el nivel supere al máximo registrado los días anteriores (2.3 metros). </v>
       </c>
     </row>
     <row r="24" spans="3:13" ht="82.5" x14ac:dyDescent="0.3">
@@ -4671,7 +4678,7 @@
       </c>
       <c r="F24" s="55" t="str">
         <f>_xlfn.CONCAT(IF(OR(MAX(CUAREIM!C17:C19)&gt;$D$3,SUM(CUAREIM!C17:C19)&gt;$E$3),$F$3,IF(OR(MAX(CUAREIM!C17:C19)&gt;$D$4,SUM(CUAREIM!C17:C19)&gt;$E$4),$F$4,$F$5)),D24,$I$3,SUM(CUAREIM!C17:C19),$J$3,MAX(CUAREIM!C17:C19),$K$3)</f>
-        <v>En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Cuareim, donde en las últimas 72 horas se acumularon 70 mm y con un máximo de 70 mm/día.</v>
+        <v>En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Cuareim, donde en las últimas 72 horas se acumularon 55.5 mm y con un máximo de 55.5 mm/día.</v>
       </c>
       <c r="G24" s="55"/>
       <c r="H24" s="55"/>
@@ -4689,7 +4696,7 @@
       </c>
       <c r="L24" s="54" t="str">
         <f t="shared" ref="L24:L30" si="0">+_xlfn.CONCAT(F24," ",I24, " ",J24," ",K24)</f>
-        <v xml:space="preserve">En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Cuareim, donde en las últimas 72 horas se acumularon 70 mm y con un máximo de 70 mm/día. Actualmente, el nivel del río Cuareim está en ascenso en la ciudad de Artigas.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  </v>
+        <v xml:space="preserve">En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Cuareim, donde en las últimas 72 horas se acumularon 55.5 mm y con un máximo de 55.5 mm/día. Actualmente, el nivel del río Cuareim está en ascenso en la ciudad de Artigas.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  </v>
       </c>
     </row>
     <row r="25" spans="3:13" ht="99" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
agregar archivos faltantes a la automatizacion qgis
</commit_message>
<xml_diff>
--- a/automatic docx/database_report.xlsx
+++ b/automatic docx/database_report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Python Scripts\automatic docx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Sala_Situacion_Dinagua\automatic docx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667CFB5F-30E3-417B-BC54-9C944185E443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA368B9-4262-4B8A-A7C0-B20E17C0AF62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{83108E16-E9D6-4CCB-B5BE-A67101359CD3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{83108E16-E9D6-4CCB-B5BE-A67101359CD3}"/>
   </bookViews>
   <sheets>
     <sheet name="INICIO" sheetId="1" r:id="rId1"/>
@@ -2109,7 +2109,7 @@
       </c>
       <c r="C3" s="42">
         <f ca="1">TODAY()</f>
-        <v>45308</v>
+        <v>45338</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -2121,7 +2121,7 @@
       </c>
       <c r="C4" s="43">
         <f ca="1">$C$3-1</f>
-        <v>45307</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2133,7 +2133,7 @@
       </c>
       <c r="C5" s="42">
         <f ca="1">$C$3-2</f>
-        <v>45306</v>
+        <v>45336</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -2145,7 +2145,7 @@
       </c>
       <c r="C6" s="43">
         <f ca="1">$C$3+1</f>
-        <v>45309</v>
+        <v>45339</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -2157,7 +2157,7 @@
       </c>
       <c r="C7" s="44">
         <f ca="1">$C$3+2</f>
-        <v>45310</v>
+        <v>45340</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2169,7 +2169,7 @@
       </c>
       <c r="C8" s="42">
         <f ca="1">$C$3+3</f>
-        <v>45311</v>
+        <v>45341</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2634,7 +2634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D9A6E30-A876-45F0-8067-30FAF0E80436}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A12" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -3577,8 +3577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2155F922-1445-4239-A643-A9F5E09853DC}">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -3725,7 +3725,7 @@
         <v>182</v>
       </c>
       <c r="C12" s="74">
-        <v>13.77</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3736,7 +3736,7 @@
         <v>183</v>
       </c>
       <c r="C13" s="73">
-        <v>13.77</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3757,9 +3757,9 @@
       <c r="B15" s="31" t="s">
         <v>184</v>
       </c>
-      <c r="C15" s="32">
+      <c r="C15" s="32" t="str">
         <f>IF((C12-C13)&gt;=0,ROUND((C12-C13)*100,0),"")</f>
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3771,7 +3771,7 @@
       </c>
       <c r="C16" s="39" t="str">
         <f>IF(C15=0,"Permanece",IF(C15="","Baja","Sube"))</f>
-        <v>Permanece</v>
+        <v>Baja</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -4748,7 +4748,7 @@
       </c>
       <c r="I26" s="66" t="str">
         <f>IF(AND(URUGUAY!$C$11=$E$8,URUGUAY!$C$16=$E$8,URUGUAY!$C$21=$E$8,URUGUAY!$C$26=$E$8),_xlfn.CONCAT($F$8,$D$26,$I$8,$J$9," ",E26,", ",E27,", ",E28," y ",Tablas!E29,"."),IF(AND(URUGUAY!$C$11=$E$9,URUGUAY!$C$16=$E$9,URUGUAY!$C$21=$E$9,URUGUAY!$C$26=$E$9),_xlfn.CONCAT($F$8,$D$26,$I$9,$J$9," ",E26,", ",E27,", ",E28," y ",E29,"."),IF(AND(URUGUAY!$C$11=$E$10,URUGUAY!$C$16=$E$10,URUGUAY!$C$21=$E$10,URUGUAY!$C$26=$E$10),_xlfn.CONCAT($F$8,$D$26,$I$10,$J$9," ",E26,", ",E27,", ",E28," y ",E29,"."),_xlfn.CONCAT($F$8,D26,I27,I28,I29))))</f>
-        <v>Actualmente, el nivel del río Uruguay está en ascenso en las ciudades de Bella Unión Paysandú; se mantiene constante en las ciudades de Salto Fray Bentos. está en descenso en la ciudad de .</v>
+        <v>Actualmente, el nivel del río Uruguay está en ascenso en las ciudades de Bella Unión Paysandú; se mantiene constante en la ciudad de  Fray Bentos; está en descenso en la ciudad de  Salto.</v>
       </c>
       <c r="J26" s="76" t="str">
         <f>_xlfn.CONCAT(F13,IF(AND(URUGUAY!C31&gt;URUGUAY!C7, URUGUAY!C33&gt;URUGUAY!C12, URUGUAY!C35&gt;URUGUAY!C17, URUGUAY!C37&gt;URUGUAY!C22),I13, IF(AND(URUGUAY!C31=URUGUAY!C7, URUGUAY!C33=URUGUAY!C12, URUGUAY!C35=URUGUAY!C17, URUGUAY!C37=URUGUAY!C22),I14, I15)))</f>
@@ -4760,7 +4760,7 @@
       </c>
       <c r="L26" s="76" t="str">
         <f t="shared" si="0"/>
-        <v>En las últimas horas se registraron bajos acumulados de precipitación en la cuenca del río Uruguay, donde en las últimas 72 horas se acumularon 0 mm y con un máximo de 0 mm/día. Actualmente, el nivel del río Uruguay está en ascenso en las ciudades de Bella Unión Paysandú; se mantiene constante en las ciudades de Salto Fray Bentos. está en descenso en la ciudad de . Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  Existe una alta probabilidad de que el nivel supere al máximo registrado los días anteriores (5m en Paysandú ).</v>
+        <v>En las últimas horas se registraron bajos acumulados de precipitación en la cuenca del río Uruguay, donde en las últimas 72 horas se acumularon 0 mm y con un máximo de 0 mm/día. Actualmente, el nivel del río Uruguay está en ascenso en las ciudades de Bella Unión Paysandú; se mantiene constante en la ciudad de  Fray Bentos; está en descenso en la ciudad de  Salto. Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  Existe una alta probabilidad de que el nivel supere al máximo registrado los días anteriores (5m en Paysandú ).</v>
       </c>
     </row>
     <row r="27" spans="3:13" ht="33" x14ac:dyDescent="0.3">
@@ -4795,15 +4795,15 @@
       <c r="F28" s="75"/>
       <c r="G28" s="60">
         <f>SUM(URUGUAY!$C$11=Tablas!E9, URUGUAY!$C$16=Tablas!E9,URUGUAY!$C$21=Tablas!E9,URUGUAY!$C$26=Tablas!E9)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H28" s="61" t="str">
         <f>_xlfn.CONCAT(IF(URUGUAY!$C$11=Tablas!E9,_xlfn.CONCAT(" ",$E$26),""),IF(URUGUAY!$C$16=Tablas!E9,_xlfn.CONCAT(" ",$E$27),""),IF(URUGUAY!$C$21=Tablas!E9,_xlfn.CONCAT(" ",$E$28),""),IF(URUGUAY!$C$26=Tablas!E9,_xlfn.CONCAT(" ",$E$29),""))</f>
-        <v xml:space="preserve"> Salto Fray Bentos</v>
+        <v xml:space="preserve"> Fray Bentos</v>
       </c>
       <c r="I28" s="67" t="str">
         <f>_xlfn.CONCAT(I9,IF(G28&gt;1,$J$9,$J$8),H28, IF((G27+G28)=4,".", ";"))</f>
-        <v xml:space="preserve"> se mantiene constante en las ciudades de Salto Fray Bentos.</v>
+        <v xml:space="preserve"> se mantiene constante en la ciudad de  Fray Bentos;</v>
       </c>
       <c r="J28" s="76"/>
       <c r="K28" s="76"/>
@@ -4818,15 +4818,15 @@
       <c r="F29" s="75"/>
       <c r="G29" s="60">
         <f>SUM(URUGUAY!$C$11=Tablas!E10, URUGUAY!$C$16=Tablas!E10,URUGUAY!$C$21=Tablas!E10,URUGUAY!$C$26=Tablas!E10)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" s="61" t="str">
         <f>_xlfn.CONCAT(IF(URUGUAY!$C$11=Tablas!E10,_xlfn.CONCAT(" ",$E$26),""),IF(URUGUAY!$C$16=Tablas!E10,_xlfn.CONCAT(" ",$E$27),""),IF(URUGUAY!$C$21=Tablas!E10,_xlfn.CONCAT(" ",$E$28),""),IF(URUGUAY!$C$26=Tablas!E10,_xlfn.CONCAT(" ",$E$29),""))</f>
-        <v/>
+        <v xml:space="preserve"> Salto</v>
       </c>
       <c r="I29" s="67" t="str">
         <f>_xlfn.CONCAT(I10,IF(G29&gt;1,$J$9,$J$8),H29, ".")</f>
-        <v xml:space="preserve"> está en descenso en la ciudad de .</v>
+        <v xml:space="preserve"> está en descenso en la ciudad de  Salto.</v>
       </c>
       <c r="J29" s="76"/>
       <c r="K29" s="76"/>

</xml_diff>

<commit_message>
update the automatic model routine with newest version
</commit_message>
<xml_diff>
--- a/automatic docx/database_report.xlsx
+++ b/automatic docx/database_report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Sala_Situacion_Dinagua\automatic docx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Python Scripts\automatic docx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA368B9-4262-4B8A-A7C0-B20E17C0AF62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A650A14E-4E5E-4BC6-9A2A-BBD2F64A0869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{83108E16-E9D6-4CCB-B5BE-A67101359CD3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{83108E16-E9D6-4CCB-B5BE-A67101359CD3}"/>
   </bookViews>
   <sheets>
     <sheet name="INICIO" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="397">
   <si>
     <t>fecha_emision</t>
   </si>
@@ -829,9 +829,6 @@
     <t xml:space="preserve">Estar atentos a los próximos eventos de lluvia que se registren en la cuenca.   </t>
   </si>
   <si>
-    <t xml:space="preserve">Estar atentos a los pronósticos meteorológicos que realiza el INUMET.   </t>
-  </si>
-  <si>
     <t xml:space="preserve">Mantener el monitoreo hidrológico reforzado en la zona y estar atento a las actualizaciones de pronósticos del tiempo para los próximos días. </t>
   </si>
   <si>
@@ -1225,16 +1222,16 @@
     <t xml:space="preserve">En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Yí, donde en las últimas 24 horas se acumularon 45.7 mm. Actualmente, el nivel del río Yí se mantiene constante en la ciudad de Durazno.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días, con una baja probabilidad de generarse afectaciones a vivienda en la ciudad de Durazno. </t>
   </si>
   <si>
-    <t>Entre 8.20 a 8.50 m</t>
-  </si>
-  <si>
-    <t>Entre 6.30 a 6.70 m</t>
-  </si>
-  <si>
     <t>18 - 19 Enero</t>
   </si>
   <si>
-    <t xml:space="preserve">En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Cuareim, donde en las últimas 24 horas se acumularon 55.5 mm. Actualmente, el nivel del río Cuareim está en ascenso en la ciudad de Artigas.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días, el cual se estima que llegue a un nivel entre 6.30 a 6.70 metros y con una bjaa probabilidad de generarse inundaciones en la zona del paseo 7 de setiembre  </t>
+    <t xml:space="preserve">En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Cuareim, donde en las últimas 72 horas se acumularon 59.6 mm y con un máximo de 49.5 mm/día. Actualmente, el nivel del río Cuareim está en ascenso en la ciudad de Artigas.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  </t>
+  </si>
+  <si>
+    <t>Entre 7.40 a 7.65 m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estar atentos a los pronósticos meteorológicos que realiza el INUMET y a los próximos eventos de lluvia que se registren en la cuenca.   </t>
   </si>
 </sst>
 </file>
@@ -2065,7 +2062,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2097,7 +2094,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="41">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2109,7 +2106,7 @@
       </c>
       <c r="C3" s="42">
         <f ca="1">TODAY()</f>
-        <v>45338</v>
+        <v>45342</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -2121,7 +2118,7 @@
       </c>
       <c r="C4" s="43">
         <f ca="1">$C$3-1</f>
-        <v>45337</v>
+        <v>45341</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2133,7 +2130,7 @@
       </c>
       <c r="C5" s="42">
         <f ca="1">$C$3-2</f>
-        <v>45336</v>
+        <v>45340</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -2145,7 +2142,7 @@
       </c>
       <c r="C6" s="43">
         <f ca="1">$C$3+1</f>
-        <v>45339</v>
+        <v>45343</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -2157,7 +2154,7 @@
       </c>
       <c r="C7" s="44">
         <f ca="1">$C$3+2</f>
-        <v>45340</v>
+        <v>45344</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2169,7 +2166,7 @@
       </c>
       <c r="C8" s="42">
         <f ca="1">$C$3+3</f>
-        <v>45341</v>
+        <v>45345</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2180,7 +2177,7 @@
         <v>174</v>
       </c>
       <c r="C9" s="45" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -2193,7 +2190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88EDC221-CFDF-4572-98F1-7407159CEFB9}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
     </sheetView>
@@ -2287,10 +2284,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
+        <v>350</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>351</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>352</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>257</v>
@@ -2344,10 +2341,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C13" s="6">
         <v>2.2999999999999998</v>
@@ -2397,10 +2394,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>345</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>346</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>257</v>
@@ -2504,7 +2501,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2515,18 +2512,18 @@
         <v>36</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>27</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2537,7 +2534,7 @@
         <v>37</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2548,7 +2545,7 @@
         <v>28</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2559,7 +2556,7 @@
         <v>38</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2570,7 +2567,7 @@
         <v>29</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2581,7 +2578,7 @@
         <v>39</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="198.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2592,10 +2589,10 @@
         <v>41</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="30" t="s">
         <v>68</v>
       </c>
@@ -2603,7 +2600,7 @@
         <v>43</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -2634,8 +2631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D9A6E30-A876-45F0-8067-30FAF0E80436}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView showGridLines="0" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2665,7 +2662,7 @@
         <v>85</v>
       </c>
       <c r="C2" s="6">
-        <v>5.6</v>
+        <v>4.6900000000000004</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2676,15 +2673,15 @@
         <v>86</v>
       </c>
       <c r="C3" s="6">
-        <v>5.75</v>
+        <v>4.71</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>345</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>346</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>257</v>
@@ -2722,7 +2719,7 @@
         <v>91</v>
       </c>
       <c r="C7" s="6">
-        <v>7.59</v>
+        <v>6.98</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2733,15 +2730,15 @@
         <v>92</v>
       </c>
       <c r="C8" s="6">
-        <v>7.1</v>
+        <v>7.21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
+        <v>346</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>347</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>348</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>257</v>
@@ -2754,9 +2751,9 @@
       <c r="B10" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="32" t="str">
         <f>IF((C7-C8)&gt;=0,ROUND((C7-C8)*100,0),"")</f>
-        <v>49</v>
+        <v/>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2768,7 +2765,7 @@
       </c>
       <c r="C11" s="39" t="str">
         <f>IF(C10=0,"Permanece",IF(C10="","Baja","Sube"))</f>
-        <v>Sube</v>
+        <v>Baja</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2779,7 +2776,7 @@
         <v>97</v>
       </c>
       <c r="C12" s="6">
-        <v>5.16</v>
+        <v>7.25</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2790,15 +2787,15 @@
         <v>98</v>
       </c>
       <c r="C13" s="6">
-        <v>4.88</v>
+        <v>7.21</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>257</v>
@@ -2813,7 +2810,7 @@
       </c>
       <c r="C15" s="32">
         <f>IF((C12-C13)&gt;=0,ROUND((C12-C13)*100,0),"")</f>
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2836,7 +2833,7 @@
         <v>77</v>
       </c>
       <c r="C17" s="8">
-        <v>55.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -2847,7 +2844,7 @@
         <v>78</v>
       </c>
       <c r="C18" s="6">
-        <v>0</v>
+        <v>49.5</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -2858,7 +2855,7 @@
         <v>79</v>
       </c>
       <c r="C19" s="6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -2869,7 +2866,7 @@
         <v>80</v>
       </c>
       <c r="C20" s="6">
-        <v>13.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -2894,14 +2891,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="28" t="s">
         <v>105</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C23" s="11"/>
     </row>
     <row r="24" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="29" t="s">
@@ -2910,7 +2906,7 @@
       <c r="B24" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C24" s="12"/>
+      <c r="C24" s="11"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="28" t="s">
@@ -2919,9 +2915,7 @@
       <c r="B25" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C25" s="11" t="s">
-        <v>394</v>
-      </c>
+      <c r="C25" s="11"/>
     </row>
     <row r="26" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="29" t="s">
@@ -2930,9 +2924,7 @@
       <c r="B26" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C26" s="12" t="s">
-        <v>387</v>
-      </c>
+      <c r="C26" s="12"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
@@ -2953,10 +2945,10 @@
         <v>102</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="215.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="28" t="s">
         <v>67</v>
       </c>
@@ -2964,7 +2956,7 @@
         <v>83</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2975,7 +2967,7 @@
         <v>84</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -3091,10 +3083,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
+        <v>334</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>335</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>336</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>257</v>
@@ -3148,10 +3140,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
+        <v>336</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>337</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>338</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>257</v>
@@ -3205,10 +3197,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>257</v>
@@ -3262,10 +3254,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
+        <v>340</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>341</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>342</v>
       </c>
       <c r="C19" s="6">
         <v>8</v>
@@ -3319,10 +3311,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
+        <v>342</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>343</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>344</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>257</v>
@@ -3536,7 +3528,7 @@
         <v>121</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3547,7 +3539,7 @@
         <v>122</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -3577,8 +3569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2155F922-1445-4239-A643-A9F5E09853DC}">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -3625,10 +3617,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
+        <v>322</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>323</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>324</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>257</v>
@@ -3683,10 +3675,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>325</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>326</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>257</v>
@@ -3725,7 +3717,7 @@
         <v>182</v>
       </c>
       <c r="C12" s="74">
-        <v>7</v>
+        <v>13.77</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3736,15 +3728,15 @@
         <v>183</v>
       </c>
       <c r="C13" s="73">
-        <v>7.1</v>
+        <v>13.77</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
+        <v>326</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>327</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>328</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>257</v>
@@ -3757,9 +3749,9 @@
       <c r="B15" s="31" t="s">
         <v>184</v>
       </c>
-      <c r="C15" s="32" t="str">
+      <c r="C15" s="32">
         <f>IF((C12-C13)&gt;=0,ROUND((C12-C13)*100,0),"")</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3771,7 +3763,7 @@
       </c>
       <c r="C16" s="39" t="str">
         <f>IF(C15=0,"Permanece",IF(C15="","Baja","Sube"))</f>
-        <v>Baja</v>
+        <v>Permanece</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3798,10 +3790,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
+        <v>328</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>329</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>330</v>
       </c>
       <c r="C19" s="6">
         <v>5</v>
@@ -3855,10 +3847,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
+        <v>330</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>331</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>332</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>257</v>
@@ -3931,7 +3923,7 @@
         <v>180</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3942,7 +3934,7 @@
         <v>175</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3953,7 +3945,7 @@
         <v>176</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -3964,7 +3956,7 @@
         <v>203</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3975,7 +3967,7 @@
         <v>204</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -3986,7 +3978,7 @@
         <v>205</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3997,7 +3989,7 @@
         <v>206</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -4019,7 +4011,7 @@
         <v>210</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="248.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4030,7 +4022,7 @@
         <v>202</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4041,7 +4033,7 @@
         <v>227</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -4072,7 +4064,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -4118,10 +4110,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
+        <v>332</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>333</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>334</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>257</v>
@@ -4175,10 +4167,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>257</v>
@@ -4315,7 +4307,7 @@
         <v>255</v>
       </c>
       <c r="C21" s="72" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4357,12 +4349,12 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="128.42578125" style="47" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="140.85546875" style="47" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11.42578125" style="47"/>
     <col min="4" max="4" width="14.85546875" style="47" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" style="47" bestFit="1" customWidth="1"/>
@@ -4381,7 +4373,7 @@
         <v>260</v>
       </c>
       <c r="C1" s="46" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D1" s="51"/>
       <c r="E1" s="51"/>
@@ -4399,26 +4391,26 @@
         <v>261</v>
       </c>
       <c r="C2" s="49" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D2" s="49" t="s">
+        <v>275</v>
+      </c>
+      <c r="E2" s="49" t="s">
         <v>276</v>
       </c>
-      <c r="E2" s="49" t="s">
-        <v>277</v>
-      </c>
       <c r="F2" s="50" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G2" s="56"/>
       <c r="H2" s="56"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
-        <v>262</v>
+        <v>396</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D3" s="47">
         <v>70</v>
@@ -4427,24 +4419,24 @@
         <v>200</v>
       </c>
       <c r="F3" s="47" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I3" s="47" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J3" s="47" t="s">
+        <v>269</v>
+      </c>
+      <c r="K3" s="47" t="s">
         <v>270</v>
-      </c>
-      <c r="K3" s="47" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D4" s="47">
         <v>30</v>
@@ -4453,20 +4445,20 @@
         <v>100</v>
       </c>
       <c r="F4" s="47" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F5" s="47" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -4474,10 +4466,10 @@
         <v>42</v>
       </c>
       <c r="E7" s="49" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F7" s="48" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G7" s="48"/>
       <c r="H7" s="48"/>
@@ -4489,49 +4481,49 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E8" s="47" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F8" s="47" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="I8" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J8" s="47" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E9" s="47" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I9" s="47" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J9" s="47" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E10" s="47" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I10" s="47" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C12" s="49" t="s">
+        <v>280</v>
+      </c>
+      <c r="D12" s="49" t="s">
+        <v>278</v>
+      </c>
+      <c r="E12" s="49" t="s">
         <v>281</v>
       </c>
-      <c r="D12" s="49" t="s">
-        <v>279</v>
-      </c>
-      <c r="E12" s="49" t="s">
-        <v>282</v>
-      </c>
       <c r="F12" s="48" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G12" s="48"/>
       <c r="H12" s="48"/>
@@ -4543,43 +4535,43 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D13" s="47" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F13" s="47" t="s">
+        <v>366</v>
+      </c>
+      <c r="I13" s="47" t="s">
         <v>367</v>
-      </c>
-      <c r="I13" s="47" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D14" s="47" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I14" s="47" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D15" s="47" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I15" s="47" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C17" s="49" t="s">
+        <v>280</v>
+      </c>
+      <c r="D17" s="49" t="s">
+        <v>278</v>
+      </c>
+      <c r="E17" s="49" t="s">
         <v>281</v>
       </c>
-      <c r="D17" s="49" t="s">
-        <v>279</v>
-      </c>
-      <c r="E17" s="49" t="s">
-        <v>282</v>
-      </c>
       <c r="F17" s="48" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G17" s="48"/>
       <c r="H17" s="48"/>
@@ -4591,57 +4583,57 @@
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.3">
       <c r="F18" s="47" t="s">
+        <v>271</v>
+      </c>
+      <c r="I18" s="47" t="s">
         <v>272</v>
-      </c>
-      <c r="I18" s="47" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="19" spans="3:13" x14ac:dyDescent="0.3">
       <c r="F19" s="47" t="s">
+        <v>273</v>
+      </c>
+      <c r="I19" s="47" t="s">
         <v>274</v>
-      </c>
-      <c r="I19" s="47" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="22" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C22" s="52" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D22" s="52" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E22" s="52" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F22" s="52" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G22" s="52"/>
       <c r="H22" s="52"/>
       <c r="I22" s="52" t="s">
+        <v>309</v>
+      </c>
+      <c r="J22" s="52" t="s">
         <v>310</v>
       </c>
-      <c r="J22" s="52" t="s">
+      <c r="K22" s="52" t="s">
         <v>311</v>
       </c>
-      <c r="K22" s="52" t="s">
-        <v>312</v>
-      </c>
       <c r="L22" s="71" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="23" spans="3:13" s="65" customFormat="1" ht="99" x14ac:dyDescent="0.25">
       <c r="C23" s="65" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D23" s="65" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E23" s="65" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F23" s="54" t="str">
         <f>_xlfn.CONCAT(IF(OR(MAX(YI!C21:C23)&gt;$D$3,SUM(YI!C21:C23)&gt;$E$3),$F$3,IF(OR(MAX(YI!C21:C23)&gt;$D$4,SUM(YI!C21:C23)&gt;$E$4),$F$4,$F$5)),D23,$I$3,SUM(YI!C21:C23),$J$3,MAX(YI!C21:C23),$K$3)</f>
@@ -4668,17 +4660,17 @@
     </row>
     <row r="24" spans="3:13" ht="82.5" x14ac:dyDescent="0.3">
       <c r="C24" s="53" t="s">
+        <v>298</v>
+      </c>
+      <c r="D24" s="53" t="s">
         <v>299</v>
       </c>
-      <c r="D24" s="53" t="s">
-        <v>300</v>
-      </c>
       <c r="E24" s="53" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F24" s="55" t="str">
         <f>_xlfn.CONCAT(IF(OR(MAX(CUAREIM!C17:C19)&gt;$D$3,SUM(CUAREIM!C17:C19)&gt;$E$3),$F$3,IF(OR(MAX(CUAREIM!C17:C19)&gt;$D$4,SUM(CUAREIM!C17:C19)&gt;$E$4),$F$4,$F$5)),D24,$I$3,SUM(CUAREIM!C17:C19),$J$3,MAX(CUAREIM!C17:C19),$K$3)</f>
-        <v>En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Cuareim, donde en las últimas 72 horas se acumularon 55.5 mm y con un máximo de 55.5 mm/día.</v>
+        <v>En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Cuareim, donde en las últimas 72 horas se acumularon 59.6 mm y con un máximo de 49.5 mm/día.</v>
       </c>
       <c r="G24" s="55"/>
       <c r="H24" s="55"/>
@@ -4696,18 +4688,18 @@
       </c>
       <c r="L24" s="54" t="str">
         <f t="shared" ref="L24:L30" si="0">+_xlfn.CONCAT(F24," ",I24, " ",J24," ",K24)</f>
-        <v xml:space="preserve">En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Cuareim, donde en las últimas 72 horas se acumularon 55.5 mm y con un máximo de 55.5 mm/día. Actualmente, el nivel del río Cuareim está en ascenso en la ciudad de Artigas.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  </v>
+        <v xml:space="preserve">En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Cuareim, donde en las últimas 72 horas se acumularon 59.6 mm y con un máximo de 49.5 mm/día. Actualmente, el nivel del río Cuareim está en ascenso en la ciudad de Artigas.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  </v>
       </c>
     </row>
     <row r="25" spans="3:13" ht="99" x14ac:dyDescent="0.3">
       <c r="C25" s="53" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E25" s="53" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F25" s="54" t="str">
         <f>_xlfn.CONCAT(IF(OR(MAX(SANTALUCIA!C27:C29)&gt;$D$3,SUM(SANTALUCIA!C27:C29)&gt;$E$3),$F$3,IF(OR(MAX(SANTALUCIA!C27:C29)&gt;$D$4,SUM(SANTALUCIA!C27:C29)&gt;$E$4),$F$4,$F$5)),D25,$I$3,SUM(SANTALUCIA!C27:C29),$J$3,MAX(SANTALUCIA!C27:C29),$K$3)</f>
@@ -4734,13 +4726,13 @@
     </row>
     <row r="26" spans="3:13" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C26" s="53" t="s">
+        <v>301</v>
+      </c>
+      <c r="D26" s="53" t="s">
         <v>302</v>
       </c>
-      <c r="D26" s="53" t="s">
+      <c r="E26" s="53" t="s">
         <v>303</v>
-      </c>
-      <c r="E26" s="53" t="s">
-        <v>304</v>
       </c>
       <c r="F26" s="75" t="str">
         <f>_xlfn.CONCAT(IF(OR(MAX(URUGUAY!C27:C29)&gt;$D$3,SUM(URUGUAY!C27:C29)&gt;$E$3),$F$3,IF(OR(MAX(URUGUAY!C27:C29)&gt;$D$4,SUM(URUGUAY!C27:C29)&gt;$E$4),$F$4,$F$5)),D26,$I$3,SUM(URUGUAY!C27:C29),$J$3,MAX(URUGUAY!C27:C29),$K$3)</f>
@@ -4748,7 +4740,7 @@
       </c>
       <c r="I26" s="66" t="str">
         <f>IF(AND(URUGUAY!$C$11=$E$8,URUGUAY!$C$16=$E$8,URUGUAY!$C$21=$E$8,URUGUAY!$C$26=$E$8),_xlfn.CONCAT($F$8,$D$26,$I$8,$J$9," ",E26,", ",E27,", ",E28," y ",Tablas!E29,"."),IF(AND(URUGUAY!$C$11=$E$9,URUGUAY!$C$16=$E$9,URUGUAY!$C$21=$E$9,URUGUAY!$C$26=$E$9),_xlfn.CONCAT($F$8,$D$26,$I$9,$J$9," ",E26,", ",E27,", ",E28," y ",E29,"."),IF(AND(URUGUAY!$C$11=$E$10,URUGUAY!$C$16=$E$10,URUGUAY!$C$21=$E$10,URUGUAY!$C$26=$E$10),_xlfn.CONCAT($F$8,$D$26,$I$10,$J$9," ",E26,", ",E27,", ",E28," y ",E29,"."),_xlfn.CONCAT($F$8,D26,I27,I28,I29))))</f>
-        <v>Actualmente, el nivel del río Uruguay está en ascenso en las ciudades de Bella Unión Paysandú; se mantiene constante en la ciudad de  Fray Bentos; está en descenso en la ciudad de  Salto.</v>
+        <v>Actualmente, el nivel del río Uruguay está en ascenso en las ciudades de Bella Unión Paysandú; se mantiene constante en las ciudades de Salto Fray Bentos. está en descenso en la ciudad de .</v>
       </c>
       <c r="J26" s="76" t="str">
         <f>_xlfn.CONCAT(F13,IF(AND(URUGUAY!C31&gt;URUGUAY!C7, URUGUAY!C33&gt;URUGUAY!C12, URUGUAY!C35&gt;URUGUAY!C17, URUGUAY!C37&gt;URUGUAY!C22),I13, IF(AND(URUGUAY!C31=URUGUAY!C7, URUGUAY!C33=URUGUAY!C12, URUGUAY!C35=URUGUAY!C17, URUGUAY!C37=URUGUAY!C22),I14, I15)))</f>
@@ -4760,14 +4752,14 @@
       </c>
       <c r="L26" s="76" t="str">
         <f t="shared" si="0"/>
-        <v>En las últimas horas se registraron bajos acumulados de precipitación en la cuenca del río Uruguay, donde en las últimas 72 horas se acumularon 0 mm y con un máximo de 0 mm/día. Actualmente, el nivel del río Uruguay está en ascenso en las ciudades de Bella Unión Paysandú; se mantiene constante en la ciudad de  Fray Bentos; está en descenso en la ciudad de  Salto. Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  Existe una alta probabilidad de que el nivel supere al máximo registrado los días anteriores (5m en Paysandú ).</v>
+        <v>En las últimas horas se registraron bajos acumulados de precipitación en la cuenca del río Uruguay, donde en las últimas 72 horas se acumularon 0 mm y con un máximo de 0 mm/día. Actualmente, el nivel del río Uruguay está en ascenso en las ciudades de Bella Unión Paysandú; se mantiene constante en las ciudades de Salto Fray Bentos. está en descenso en la ciudad de . Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  Existe una alta probabilidad de que el nivel supere al máximo registrado los días anteriores (5m en Paysandú ).</v>
       </c>
     </row>
     <row r="27" spans="3:13" ht="33" x14ac:dyDescent="0.3">
       <c r="C27" s="53"/>
       <c r="D27" s="53"/>
       <c r="E27" s="53" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F27" s="75"/>
       <c r="G27" s="60">
@@ -4790,20 +4782,20 @@
       <c r="C28" s="53"/>
       <c r="D28" s="53"/>
       <c r="E28" s="53" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F28" s="75"/>
       <c r="G28" s="60">
         <f>SUM(URUGUAY!$C$11=Tablas!E9, URUGUAY!$C$16=Tablas!E9,URUGUAY!$C$21=Tablas!E9,URUGUAY!$C$26=Tablas!E9)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H28" s="61" t="str">
         <f>_xlfn.CONCAT(IF(URUGUAY!$C$11=Tablas!E9,_xlfn.CONCAT(" ",$E$26),""),IF(URUGUAY!$C$16=Tablas!E9,_xlfn.CONCAT(" ",$E$27),""),IF(URUGUAY!$C$21=Tablas!E9,_xlfn.CONCAT(" ",$E$28),""),IF(URUGUAY!$C$26=Tablas!E9,_xlfn.CONCAT(" ",$E$29),""))</f>
-        <v xml:space="preserve"> Fray Bentos</v>
+        <v xml:space="preserve"> Salto Fray Bentos</v>
       </c>
       <c r="I28" s="67" t="str">
         <f>_xlfn.CONCAT(I9,IF(G28&gt;1,$J$9,$J$8),H28, IF((G27+G28)=4,".", ";"))</f>
-        <v xml:space="preserve"> se mantiene constante en la ciudad de  Fray Bentos;</v>
+        <v xml:space="preserve"> se mantiene constante en las ciudades de Salto Fray Bentos.</v>
       </c>
       <c r="J28" s="76"/>
       <c r="K28" s="76"/>
@@ -4813,20 +4805,20 @@
       <c r="C29" s="53"/>
       <c r="D29" s="53"/>
       <c r="E29" s="53" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F29" s="75"/>
       <c r="G29" s="60">
         <f>SUM(URUGUAY!$C$11=Tablas!E10, URUGUAY!$C$16=Tablas!E10,URUGUAY!$C$21=Tablas!E10,URUGUAY!$C$26=Tablas!E10)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H29" s="61" t="str">
         <f>_xlfn.CONCAT(IF(URUGUAY!$C$11=Tablas!E10,_xlfn.CONCAT(" ",$E$26),""),IF(URUGUAY!$C$16=Tablas!E10,_xlfn.CONCAT(" ",$E$27),""),IF(URUGUAY!$C$21=Tablas!E10,_xlfn.CONCAT(" ",$E$28),""),IF(URUGUAY!$C$26=Tablas!E10,_xlfn.CONCAT(" ",$E$29),""))</f>
-        <v xml:space="preserve"> Salto</v>
+        <v/>
       </c>
       <c r="I29" s="67" t="str">
         <f>_xlfn.CONCAT(I10,IF(G29&gt;1,$J$9,$J$8),H29, ".")</f>
-        <v xml:space="preserve"> está en descenso en la ciudad de  Salto.</v>
+        <v xml:space="preserve"> está en descenso en la ciudad de .</v>
       </c>
       <c r="J29" s="76"/>
       <c r="K29" s="76"/>
@@ -4834,13 +4826,13 @@
     </row>
     <row r="30" spans="3:13" ht="82.5" x14ac:dyDescent="0.3">
       <c r="C30" s="53" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D30" s="53" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E30" s="53" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F30" s="54" t="str">
         <f>_xlfn.CONCAT(IF(OR(MAX(NEGRO!C12:C14)&gt;$D$3,SUM(NEGRO!C12:C14)&gt;$E$3),$F$3,IF(OR(MAX(NEGRO!C12:C14)&gt;$D$4,SUM(NEGRO!C12:C14)&gt;$E$4),$F$4,$F$5)),D30,$I$3,SUM(NEGRO!C12:C14),$J$3,MAX(NEGRO!C12:C14),$K$3)</f>
@@ -4899,16 +4891,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="s">
+        <v>354</v>
+      </c>
+      <c r="B1" s="59" t="s">
         <v>355</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="C1" s="62" t="s">
         <v>356</v>
       </c>
-      <c r="C1" s="62" t="s">
-        <v>357</v>
-      </c>
       <c r="D1" s="62" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4916,13 +4908,13 @@
         <v>45224</v>
       </c>
       <c r="B2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C2" s="63" t="s">
         <v>358</v>
       </c>
-      <c r="C2" s="63" t="s">
-        <v>359</v>
-      </c>
       <c r="D2" s="63" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -4930,10 +4922,10 @@
         <v>45224</v>
       </c>
       <c r="B3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C3" s="63" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -4941,13 +4933,13 @@
         <v>45224</v>
       </c>
       <c r="B4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C4" s="63" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D4" s="63" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4955,10 +4947,10 @@
         <v>45224</v>
       </c>
       <c r="B5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C5" s="63" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4966,10 +4958,10 @@
         <v>45224</v>
       </c>
       <c r="B6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D6" s="64" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4977,13 +4969,13 @@
         <v>45224</v>
       </c>
       <c r="B7" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C7" s="63" t="s">
+        <v>372</v>
+      </c>
+      <c r="D7" s="63" t="s">
         <v>373</v>
-      </c>
-      <c r="D7" s="63" t="s">
-        <v>374</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
include Olimar report in the flood report generator
</commit_message>
<xml_diff>
--- a/automatic docx/database_report.xlsx
+++ b/automatic docx/database_report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Python Scripts\automatic docx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A650A14E-4E5E-4BC6-9A2A-BBD2F64A0869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221577AB-5914-45F0-B1B9-6FC7266232AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{83108E16-E9D6-4CCB-B5BE-A67101359CD3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{83108E16-E9D6-4CCB-B5BE-A67101359CD3}"/>
   </bookViews>
   <sheets>
     <sheet name="INICIO" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,9 @@
     <sheet name="SANTALUCIA" sheetId="5" r:id="rId4"/>
     <sheet name="URUGUAY" sheetId="7" r:id="rId5"/>
     <sheet name="NEGRO" sheetId="6" r:id="rId6"/>
-    <sheet name="Tablas" sheetId="8" r:id="rId7"/>
-    <sheet name="log" sheetId="9" r:id="rId8"/>
+    <sheet name="OLIMAR" sheetId="10" r:id="rId7"/>
+    <sheet name="Tablas" sheetId="8" r:id="rId8"/>
+    <sheet name="log" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="421">
   <si>
     <t>fecha_emision</t>
   </si>
@@ -148,9 +149,6 @@
     <t>fecha_pronos_72</t>
   </si>
   <si>
-    <t>Entre 8.5 a 9.5 m</t>
-  </si>
-  <si>
     <t>fecha_sarandi</t>
   </si>
   <si>
@@ -163,9 +161,6 @@
     <t>fecha_nuevo</t>
   </si>
   <si>
-    <t>29 - 30 oct</t>
-  </si>
-  <si>
     <t>diagnostico_yi</t>
   </si>
   <si>
@@ -817,12 +812,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>15,000 a 17,000</t>
-  </si>
-  <si>
-    <t>9,000 a 10,000</t>
-  </si>
-  <si>
     <t>Recomendaciones al SINAE</t>
   </si>
   <si>
@@ -1168,70 +1157,154 @@
     <t>Frase completa</t>
   </si>
   <si>
-    <t>En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Santa Lucía, donde en las últimas 72 horas se acumularon 105 mm y con un máximo de 35 mm/día. Actualmente, el nivel del río Santa Lucía está en ascenso en la ciudad de Santa Lucía.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  Existe una baja probabilidad de que el nivel supere al máximo registrado los días anteriores (8 metros), pero no se puede descartar en su totalidad.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En las últimas horas se registraron importantes acumulados de precipitación en la cuenca del Río Negro, donde en las últimas 72 horas se acumularon 210 mm y con un máximo de 70 mm/día. Actualmente, el nivel del Río Negro está en ascenso en la ciudad de Mercedes.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  </t>
-  </si>
-  <si>
-    <t>24,000 y 25,000</t>
-  </si>
-  <si>
-    <t>Entre 8.90 a 9.10</t>
-  </si>
-  <si>
-    <t>28 - 29 oct</t>
-  </si>
-  <si>
-    <t>Entre 14.00 y 14.20</t>
-  </si>
-  <si>
-    <t>Entre 7.30 a 7.70</t>
-  </si>
-  <si>
-    <t>En las últimas horas se registraron bajos acumulados de precipitación en la cuenca del río Uruguay, donde en las últimas 72 horas se acumularon 0 mm y con un máximo de 0 mm/día. Actualmente, el nivel del río Uruguay está en ascenso en las ciudades de Bella Unión Paysandú; se mantiene constante en las ciudades de Salto Fray Bentos. está en descenso en la ciudad de . Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  Existe una alta probabilidad de que el nivel supere al máximo registrado los días anteriores (5m en Paysandú ).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estar atentos a posibles inundaciones locales en la zona del paseo 7 de setiembre. </t>
-  </si>
-  <si>
-    <t>Se registra incrementos del río Cuareim en Artigas con baja posibilidad de afectar la zona del paseo 7 de setiembre</t>
-  </si>
-  <si>
-    <t>Menor a 2.0 m</t>
-  </si>
-  <si>
-    <t>17 - 18 Enero</t>
-  </si>
-  <si>
-    <t>18 - 20 Enero</t>
-  </si>
-  <si>
-    <t>Menor a 5.0 m</t>
-  </si>
-  <si>
-    <t>Menor a 3.5 m</t>
-  </si>
-  <si>
-    <t>19 - 21 Enero</t>
-  </si>
-  <si>
-    <t>Menor a 5.9 m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Yí, donde en las últimas 24 horas se acumularon 45.7 mm. Actualmente, el nivel del río Yí se mantiene constante en la ciudad de Durazno.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días, con una baja probabilidad de generarse afectaciones a vivienda en la ciudad de Durazno. </t>
-  </si>
-  <si>
-    <t>18 - 19 Enero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Cuareim, donde en las últimas 72 horas se acumularon 59.6 mm y con un máximo de 49.5 mm/día. Actualmente, el nivel del río Cuareim está en ascenso en la ciudad de Artigas.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  </t>
-  </si>
-  <si>
-    <t>Entre 7.40 a 7.65 m</t>
-  </si>
-  <si>
     <t xml:space="preserve">Estar atentos a los pronósticos meteorológicos que realiza el INUMET y a los próximos eventos de lluvia que se registren en la cuenca.   </t>
+  </si>
+  <si>
+    <t>Entre 9.0 a 9.5 m</t>
+  </si>
+  <si>
+    <t>30 mayo</t>
+  </si>
+  <si>
+    <t>02 - 03 mayo</t>
+  </si>
+  <si>
+    <t>Entre 9.8 - 9.3 m</t>
+  </si>
+  <si>
+    <t>Entre 8.2 a 8.6 m</t>
+  </si>
+  <si>
+    <t>Estar preparados ante la posibilidad de inundaciones que afecten a zona de vivienda.</t>
+  </si>
+  <si>
+    <t>Menor a 8.5 m</t>
+  </si>
+  <si>
+    <t>Entre 29 - 30 mayo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29 mayo </t>
+  </si>
+  <si>
+    <t>29 - 30 mayo</t>
+  </si>
+  <si>
+    <t>10 mm en la parte alta de la cuenca</t>
+  </si>
+  <si>
+    <t>4 mm en la parte alta de la cuenca</t>
+  </si>
+  <si>
+    <t>35.8 mm en Alto río Negro</t>
+  </si>
+  <si>
+    <t>Menor a 3600</t>
+  </si>
+  <si>
+    <t>Menor a 4578</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estar atentos a los incrementos de nivel del río Negro en el tramo Represa Constitución y Mercedes. </t>
+  </si>
+  <si>
+    <t>Se mantienen los incrementos de nivel en los ríos Yí y Santa Lucía.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actualmente se encuentra en tránsito una crecida del río Yí en el tramo Polanco del Yí y Durazno. En Sarandí Yí se registró el dia de ayer un nivel máximo de 5.44 m y actualmente se encuentra en descenso. En Polanco del Yí se encuentra en ascenso el nivel del río en una cota de 8.39 m (3 cm/h). En Durazno puente viejo se tiene un nivel de 9.14 m (Puente Ruta 5) y 8.05 m (en Puente Viejo). Estos niveles estan en ascenso y aun por debajo de la cota de seguridad (8.2 m en Durazno Puente Viejo). En base a estas condiciones se espera que se mantenga en ascenso el nivel del río Yí y superando la cota de seguridad en el transcurso del día. Actualmente el nivel máximo pronosticado para Durazno seria entre 8.2 a 8.6 metros en Durazno puente viejo para 02 o 03 de mayo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">En las últimas horas no se registraron precipitaciones en la cuenca del río Cuareim. Actualmente, el nivel del río Cuareim se mantiene constante en la ciudad de Artigas.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, se prevé que el nivel siga en descenso en los próximos días.  </t>
+  </si>
+  <si>
+    <t>Menor a 4.0 m</t>
+  </si>
+  <si>
+    <t>Menor a 5.50 m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se encuentra en ascenso el nivel del río Santa Lucia en Ruta 11 (7.61 m), Aguas corrientes (5.17 m). OSE reporta que el nivel del embalse Paso severino es de 38.94 m. De acuerdo a la información brindada el día de ayer, se espera que en el transcurso de este día y mañana se tenga el nivel máximo del río Santa Lucia en Ruta 11, llegando a un nivel menor a 8.5 m y por debajo levemente de la cota de seguridad (9.36 m). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estar atentos a los incrementos de nivel que está experimentando el río Santa Lucia. </t>
+  </si>
+  <si>
+    <t>entre 12,800 y 13,800</t>
+  </si>
+  <si>
+    <t>En las últimas horas se registraron bajos acumulados de precipitación en la cuenca del río Uruguay. Actualmente el nivel del río se mantiene con un descenso de nivel en el tramo Salto - Fray Bentos. Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, se prevé que se mantega la tendencia descendiente.</t>
+  </si>
+  <si>
+    <t>5.91 m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En las últimas horas no se registraron precipitaciones significativas en la cuenca del río Negro. UTE reporta que el nivel del río Negro en San Gregorio de Polanco podria descender los próximos dias, mientras que en Mercedes se espera para el 30-05-2024 un incremento de nivel que llegaria a un nivel de 5.91 m. </t>
+  </si>
+  <si>
+    <t>último dato en Treinta y Tres</t>
+  </si>
+  <si>
+    <t>anterior dato en Treinta y Tres (1 hora)</t>
+  </si>
+  <si>
+    <t>nivel pico anterior en Treinta y Tres</t>
+  </si>
+  <si>
+    <t>Pronostico hidrologico en Treinta y Tres</t>
+  </si>
+  <si>
+    <t>fecha ocurrencia nivel máximo en Treinta y Tres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Yí, donde en las últimas 72 horas se acumularon 63.8 mm y con un máximo de 63.8 mm/día. Actualmente, el nivel del río Yí está en ascenso en la ciudad de Durazno.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  Existe una alta probabilidad de que el nivel supere al máximo registrado los días anteriores ( metros). </t>
+  </si>
+  <si>
+    <t>nivel_actual_treintatres</t>
+  </si>
+  <si>
+    <t>nivel_pasado_treintatres</t>
+  </si>
+  <si>
+    <t>nivel_pico_anterior_treintatres</t>
+  </si>
+  <si>
+    <t>tasa_treintatres</t>
+  </si>
+  <si>
+    <t>tendencia_treintatres</t>
+  </si>
+  <si>
+    <t>pobs_24_olimar</t>
+  </si>
+  <si>
+    <t>pobs_48_olimar</t>
+  </si>
+  <si>
+    <t>pobs_72_olimar</t>
+  </si>
+  <si>
+    <t>psim_24_olimar</t>
+  </si>
+  <si>
+    <t>psim_48_olimar</t>
+  </si>
+  <si>
+    <t>psim_72_olimar</t>
+  </si>
+  <si>
+    <t>fecha_treintatres</t>
+  </si>
+  <si>
+    <t>pronos_treintatres</t>
+  </si>
+  <si>
+    <t>diagnostico_olimar</t>
+  </si>
+  <si>
+    <t>recomendacion_olimar</t>
+  </si>
+  <si>
+    <t>30 Octubre</t>
   </si>
 </sst>
 </file>
@@ -1527,7 +1600,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1737,6 +1810,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2062,7 +2138,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2077,7 +2153,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>9</v>
@@ -2088,96 +2164,96 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="41">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="23" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B3" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="42">
         <f ca="1">TODAY()</f>
-        <v>45342</v>
+        <v>45593</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B4" s="34" t="s">
         <v>31</v>
       </c>
       <c r="C4" s="43">
         <f ca="1">$C$3-1</f>
-        <v>45341</v>
+        <v>45592</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B5" s="33" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="42">
         <f ca="1">$C$3-2</f>
-        <v>45340</v>
+        <v>45591</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B6" s="34" t="s">
         <v>32</v>
       </c>
       <c r="C6" s="43">
         <f ca="1">$C$3+1</f>
-        <v>45343</v>
+        <v>45594</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B7" s="35" t="s">
         <v>33</v>
       </c>
       <c r="C7" s="44">
         <f ca="1">$C$3+2</f>
-        <v>45344</v>
+        <v>45595</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B8" s="33" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="42">
         <f ca="1">$C$3+3</f>
-        <v>45345</v>
+        <v>45596</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="21" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C9" s="45" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -2190,14 +2266,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88EDC221-CFDF-4572-98F1-7407159CEFB9}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.28515625" style="16" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="48.28515625" style="5" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="5"/>
@@ -2205,7 +2281,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>9</v>
@@ -2216,242 +2292,242 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="8">
-        <v>1.17</v>
+      <c r="C2" s="74">
+        <v>4.67</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6">
-        <v>1.17</v>
+      <c r="C3" s="73">
+        <v>4.72</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="32">
-        <f>IFERROR(ROUND(ABS(C2-C3)*100,0),"-")</f>
-        <v>0</v>
+      <c r="C4" s="32" t="str">
+        <f>IF((C2-C3)&gt;=0,ROUND((C2-C3)*100,0),"")</f>
+        <v/>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5" s="38" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="39" t="str">
-        <f>IFERROR(IF(C4=0,"Permanece",IF(SIGN(C4)=1,"Sube","Baja")),"-")</f>
-        <v>Permanece</v>
+        <f>IF(C4=0,"Permanece",IF(C4="","Baja","Sube"))</f>
+        <v>Baja</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="8">
-        <v>2.0499999999999998</v>
+      <c r="C6" s="74">
+        <v>8.39</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6">
-        <v>2.0499999999999998</v>
+      <c r="C7" s="73">
+        <v>8.36</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B9" s="31" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="32">
         <f>IF((C6-C7)&gt;=0,ROUND((C6-C7)*100,0),"")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B10" s="38" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="39" t="str">
         <f>IF(C9=0,"Permanece",IF(C9="","Baja","Sube"))</f>
-        <v>Permanece</v>
+        <v>Sube</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="8">
-        <v>0.26</v>
+      <c r="C11" s="74">
+        <v>8.0500000000000007</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="6">
-        <v>0.26</v>
+      <c r="C12" s="73">
+        <v>8.01</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>352</v>
-      </c>
-      <c r="C13" s="6">
-        <v>2.2999999999999998</v>
-      </c>
+        <v>348</v>
+      </c>
+      <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B14" s="31" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="32">
         <f>IF((C11-C12)&gt;=0,ROUND((C11-C12)*100,0),"")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B15" s="38" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="39" t="str">
         <f>IF(C14=0,"Permanece",IF(C14="","Baja","Sube"))</f>
-        <v>Permanece</v>
+        <v>Sube</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="6"/>
+      <c r="C16" s="73">
+        <v>9.14</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="6"/>
+      <c r="C17" s="73">
+        <v>9.1</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>345</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>257</v>
-      </c>
+        <v>341</v>
+      </c>
+      <c r="C18" s="6"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B19" s="31" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="32">
         <f>IF((C16-C17)&gt;=0,ROUND((C16-C17)*100,0),"")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B20" s="38" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="39" t="str">
         <f>IF(C19=0,"Permanece",IF(C19="","Baja","Sube"))</f>
-        <v>Permanece</v>
+        <v>Sube</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="8">
-        <v>45.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="6">
-        <v>2</v>
+        <v>63.8</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>22</v>
@@ -2462,7 +2538,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>23</v>
@@ -2473,18 +2549,18 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C25" s="6">
-        <v>4.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>25</v>
@@ -2495,112 +2571,108 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="11" t="s">
-        <v>385</v>
-      </c>
+      <c r="C27" s="11"/>
     </row>
     <row r="28" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>386</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C28" s="12"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>27</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>389</v>
+        <v>372</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>28</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>388</v>
+        <v>376</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="29" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>390</v>
+        <v>374</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>391</v>
+        <v>375</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="281.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="198.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="B35" s="7" t="s">
+      <c r="B36" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C35" s="13" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="B36" s="14" t="s">
-        <v>43</v>
-      </c>
       <c r="C36" s="15" t="s">
-        <v>263</v>
+        <v>377</v>
       </c>
     </row>
   </sheetData>
@@ -2631,8 +2703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D9A6E30-A876-45F0-8067-30FAF0E80436}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView showGridLines="0" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2645,7 +2717,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>9</v>
@@ -2656,214 +2728,214 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C2" s="6">
-        <v>4.6900000000000004</v>
+        <v>4.2300000000000004</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C3" s="6">
-        <v>4.71</v>
+        <v>4.2300000000000004</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="C5" s="32" t="str">
+        <v>85</v>
+      </c>
+      <c r="C5" s="32">
         <f>IF((C2-C3)&gt;=0,ROUND((C2-C3)*100,0),"")</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C6" s="39" t="str">
         <f>IF(C5=0,"Permanece",IF(C5="","Baja","Sube"))</f>
-        <v>Baja</v>
+        <v>Permanece</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C7" s="6">
-        <v>6.98</v>
+        <v>1.53</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C8" s="6">
-        <v>7.21</v>
+        <v>1.53</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>93</v>
-      </c>
-      <c r="C10" s="32" t="str">
+        <v>91</v>
+      </c>
+      <c r="C10" s="32">
         <f>IF((C7-C8)&gt;=0,ROUND((C7-C8)*100,0),"")</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C11" s="39" t="str">
         <f>IF(C10=0,"Permanece",IF(C10="","Baja","Sube"))</f>
-        <v>Baja</v>
+        <v>Permanece</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C12" s="6">
-        <v>7.25</v>
+        <v>2.56</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C13" s="6">
-        <v>7.21</v>
+        <v>2.56</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C15" s="32">
         <f>IF((C12-C13)&gt;=0,ROUND((C12-C13)*100,0),"")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C16" s="39" t="str">
         <f>IF(C15=0,"Permanece",IF(C15="","Baja","Sube"))</f>
-        <v>Sube</v>
+        <v>Permanece</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C17" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C18" s="6">
-        <v>49.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C19" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C20" s="6">
         <v>0</v>
@@ -2871,10 +2943,10 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C21" s="6">
         <v>0</v>
@@ -2882,10 +2954,10 @@
     </row>
     <row r="22" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C22" s="10">
         <v>0</v>
@@ -2893,81 +2965,78 @@
     </row>
     <row r="23" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="28" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>89</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="C23" s="75"/>
     </row>
     <row r="24" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="29" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C24" s="11"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="28" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C25" s="11"/>
     </row>
     <row r="26" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="29" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="C26" s="12"/>
+        <v>94</v>
+      </c>
+      <c r="C26" s="11"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>395</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="C27" s="11"/>
     </row>
     <row r="28" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="29" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="C28" s="12"/>
+    </row>
+    <row r="29" spans="1:11" ht="132.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>383</v>
+        <v>257</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -3037,7 +3106,7 @@
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B38" sqref="B1:B1048576"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -3050,7 +3119,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>9</v>
@@ -3061,226 +3130,214 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C2" s="8">
-        <v>6.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="C3" s="6">
-        <v>6.1</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C5" s="32">
         <f>IF((C2-C3)&gt;=0,ROUND((C2-C3)*100,0),"")</f>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C6" s="39" t="str">
         <f>IF(C5=0,"Permanece",IF(C5="","Baja","Sube"))</f>
-        <v>Permanece</v>
+        <v>Sube</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="C7" s="8">
-        <v>5.4</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="C7" s="8"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C8" s="6">
-        <v>5.2</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C10" s="32">
         <f>IF((C7-C8)&gt;=0,ROUND((C7-C8)*100,0),"")</f>
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C11" s="39" t="str">
         <f>IF(C10=0,"Permanece",IF(C10="","Baja","Sube"))</f>
-        <v>Sube</v>
+        <v>Permanece</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="C12" s="8">
-        <v>5.4</v>
-      </c>
+      <c r="C12" s="8"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="C13" s="6">
-        <v>5.2</v>
-      </c>
+      <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C15" s="32">
         <f>IF((C12-C13)&gt;=0,ROUND((C12-C13)*100,0),"")</f>
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B16" s="38" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C16" s="39" t="str">
         <f>IF(C15=0,"Permanece",IF(C15="","Baja","Sube"))</f>
-        <v>Sube</v>
+        <v>Permanece</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C17" s="8">
-        <v>2.1</v>
+        <v>7.91</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C18" s="6">
-        <v>1.9</v>
+        <v>7.86</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>341</v>
-      </c>
-      <c r="C19" s="6">
-        <v>8</v>
-      </c>
+        <v>337</v>
+      </c>
+      <c r="C19" s="6"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C20" s="32">
         <f>IF((C17-C18)&gt;=0,ROUND((C17-C18)*100,0),"")</f>
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B21" s="38" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C21" s="39" t="str">
         <f>IF(C20=0,"Permanece",IF(C20="","Baja","Sube"))</f>
@@ -3289,257 +3346,243 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>257</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="C22" s="6"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>257</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="C23" s="6"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>343</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>257</v>
-      </c>
+        <v>339</v>
+      </c>
+      <c r="C24" s="6"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B25" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="C25" s="32" t="str">
+        <v>133</v>
+      </c>
+      <c r="C25" s="32">
         <f>IFERROR(ROUND(ABS(C22-C23)*100,0),"-")</f>
-        <v>-</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B26" s="38" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C26" s="39" t="str">
         <f>IFERROR(IF(C25=0,"Permanece",IF(SIGN(C25)=1,"Sube","Baja")),"-")</f>
-        <v>-</v>
+        <v>Permanece</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C27" s="8">
-        <v>35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C28" s="6">
-        <v>35</v>
+        <v>55.9</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C29" s="10">
-        <v>35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C30" s="6">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C31" s="6">
-        <v>80</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C32" s="10">
-        <v>65</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="28" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="C33" s="11">
-        <v>7.2</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="C33" s="11"/>
     </row>
     <row r="34" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="29" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>40</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="C34" s="12"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="28" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="C35" s="11">
-        <v>8.9</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="C35" s="11"/>
     </row>
     <row r="36" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="29" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>40</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="C36" s="12"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C37" s="11">
-        <v>8.9</v>
+      <c r="C37" s="11" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>164</v>
-      </c>
       <c r="C38" s="12" t="s">
-        <v>40</v>
+        <v>381</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="28" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="C39" s="11">
-        <v>7.2</v>
+        <v>129</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="29" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>40</v>
+        <v>379</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="28" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>35</v>
+        <v>392</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="29" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="231.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>262</v>
+        <v>394</v>
       </c>
     </row>
   </sheetData>
@@ -3569,8 +3612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2155F922-1445-4239-A643-A9F5E09853DC}">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -3584,7 +3627,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>9</v>
@@ -3595,159 +3638,159 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C2" s="74">
-        <v>11.34</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C3" s="73">
-        <v>11.34</v>
+        <v>7.78</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C5" s="32">
         <f>IF((C2-C3)&gt;=0,ROUND((C2-C3)*100,0),"")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D5" s="57"/>
     </row>
     <row r="6" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C6" s="39" t="str">
         <f>IF(C5=0,"Permanece",IF(C5="","Baja","Sube"))</f>
-        <v>Permanece</v>
+        <v>Sube</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C7" s="74">
-        <v>8.9700000000000006</v>
+        <v>5.65</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C8" s="73">
-        <v>8.9499999999999993</v>
+        <v>5.65</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C10" s="32">
         <f>IF((C7-C8)&gt;=0,ROUND((C7-C8)*100,0),"")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D10" s="57"/>
     </row>
     <row r="11" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C11" s="39" t="str">
         <f>IF(C10=0,"Permanece",IF(C10="","Baja","Sube"))</f>
-        <v>Sube</v>
+        <v>Permanece</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C12" s="74">
-        <v>13.77</v>
+        <v>9.73</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C13" s="73">
-        <v>13.77</v>
+        <v>9.73</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C15" s="32">
         <f>IF((C12-C13)&gt;=0,ROUND((C12-C13)*100,0),"")</f>
@@ -3756,10 +3799,10 @@
     </row>
     <row r="16" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C16" s="39" t="str">
         <f>IF(C15=0,"Permanece",IF(C15="","Baja","Sube"))</f>
@@ -3768,126 +3811,126 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C17" s="74">
-        <v>7.22</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C18" s="73">
-        <v>7.21</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C19" s="6">
-        <v>5</v>
+        <v>7.89</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C20" s="32">
         <f>IF((C17-C18)&gt;=0,ROUND((C17-C18)*100,0),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B21" s="38" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C21" s="39" t="str">
         <f>IF(C20=0,"Permanece",IF(C20="","Baja","Sube"))</f>
-        <v>Sube</v>
+        <v>Permanece</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="28" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C22" s="74">
-        <v>2.89</v>
+        <v>2.78</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C23" s="73">
-        <v>2.89</v>
+        <v>2.88</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B25" s="31" t="s">
-        <v>225</v>
-      </c>
-      <c r="C25" s="32">
+        <v>223</v>
+      </c>
+      <c r="C25" s="32" t="str">
         <f>IF((C22-C23)&gt;=0,ROUND((C22-C23)*100,0),"")</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D25" s="57"/>
     </row>
     <row r="26" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B26" s="38" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C26" s="39" t="str">
         <f>IF(C25=0,"Permanece",IF(C25="","Baja","Sube"))</f>
-        <v>Permanece</v>
+        <v>Baja</v>
       </c>
       <c r="D26" s="57"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C27" s="8">
         <v>0</v>
@@ -3895,145 +3938,129 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="C28" s="6">
-        <v>0</v>
+        <v>176</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="C29" s="6">
-        <v>0</v>
+        <v>177</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="27" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>377</v>
+        <v>395</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="28" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>378</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="C31" s="11"/>
     </row>
     <row r="32" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="29" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>379</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="C32" s="12"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>380</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="C33" s="11"/>
     </row>
     <row r="34" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="29" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>379</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="C34" s="12"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="28" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>381</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="C35" s="11"/>
     </row>
     <row r="36" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="29" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>379</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="C36" s="12"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="B37" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="B37" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="C37" s="11">
-        <v>3.4</v>
-      </c>
+      <c r="C37" s="11"/>
     </row>
     <row r="38" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="B38" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="B38" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="248.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="12"/>
+    </row>
+    <row r="39" spans="1:3" ht="132.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -4063,8 +4090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7698158D-7CF5-4621-99AA-4EF5CEB60D57}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -4077,7 +4104,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>9</v>
@@ -4088,237 +4115,233 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
+        <v>226</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>230</v>
-      </c>
       <c r="C2" s="8">
-        <v>6.1</v>
+        <v>11.65</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>231</v>
-      </c>
       <c r="C3" s="6">
-        <v>6.1</v>
+        <v>11.64</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C5" s="32">
         <f>IF((C2-C3)&gt;=0,ROUND((C2-C3)*100,0),"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C6" s="39" t="str">
         <f>IF(C5=0,"Permanece",IF(C5="","Baja","Sube"))</f>
-        <v>Permanece</v>
+        <v>Sube</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
+        <v>232</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>236</v>
-      </c>
       <c r="C7" s="8">
-        <v>5.4</v>
+        <v>5.87</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>237</v>
-      </c>
       <c r="C8" s="6">
-        <v>5.2</v>
+        <v>5.87</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C10" s="32">
         <f>IF((C7-C8)&gt;=0,ROUND((C7-C8)*100,0),"")</f>
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C11" s="39" t="str">
         <f>IF(C10=0,"Permanece",IF(C10="","Baja","Sube"))</f>
-        <v>Sube</v>
+        <v>Permanece</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C12" s="8">
-        <v>70</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="C13" s="6">
-        <v>70</v>
+        <v>239</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C14" s="6">
-        <v>70</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>259</v>
+        <v>385</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="27" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>258</v>
+        <v>386</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
+        <v>249</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="C17" s="11">
-        <v>8.9</v>
-      </c>
+      <c r="C17" s="11"/>
     </row>
     <row r="18" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29" t="s">
+        <v>250</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>40</v>
-      </c>
+      <c r="C18" s="12"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>247</v>
-      </c>
-      <c r="C19" s="11">
-        <v>7.2</v>
+        <v>245</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="29" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="132.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C21" s="72" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>261</v>
+        <v>387</v>
       </c>
     </row>
   </sheetData>
@@ -4345,6 +4368,225 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F4874F4-C602-4D36-9B06-CCCD4B9EE49C}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" style="16" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="48.28515625" style="5" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>399</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="C2" s="74">
+        <v>8.39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
+        <v>400</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="C3" s="73">
+        <v>8.36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
+        <v>401</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>408</v>
+      </c>
+      <c r="C5" s="32">
+        <f>IF((C2-C3)&gt;=0,ROUND((C2-C3)*100,0),"")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>409</v>
+      </c>
+      <c r="C6" s="39" t="str">
+        <f>IF(C5=0,"Permanece",IF(C5="","Baja","Sube"))</f>
+        <v>Sube</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="C8" s="6">
+        <v>63.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="C12" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>402</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="C13" s="11">
+        <v>7.24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>416</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="198.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>419</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>377</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{E0C1EDD8-69C1-437F-95B8-A9746EDF6452}">
+          <x14:formula1>
+            <xm:f>Tablas!$L$23</xm:f>
+          </x14:formula1>
+          <xm:sqref>C15</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{26980350-1545-428A-98A8-01DCC1E0202D}">
+          <x14:formula1>
+            <xm:f>Tablas!$A$2:$A$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>C16</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F783B566-6E24-4EBC-9E3F-D2E3A05600BD}">
   <dimension ref="A1:M30"/>
   <sheetViews>
@@ -4370,10 +4612,10 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C1" s="46" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D1" s="51"/>
       <c r="E1" s="51"/>
@@ -4388,29 +4630,29 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
+        <v>257</v>
+      </c>
+      <c r="C2" s="49" t="s">
+        <v>274</v>
+      </c>
+      <c r="D2" s="49" t="s">
+        <v>271</v>
+      </c>
+      <c r="E2" s="49" t="s">
+        <v>272</v>
+      </c>
+      <c r="F2" s="50" t="s">
         <v>261</v>
-      </c>
-      <c r="C2" s="49" t="s">
-        <v>278</v>
-      </c>
-      <c r="D2" s="49" t="s">
-        <v>275</v>
-      </c>
-      <c r="E2" s="49" t="s">
-        <v>276</v>
-      </c>
-      <c r="F2" s="50" t="s">
-        <v>265</v>
       </c>
       <c r="G2" s="56"/>
       <c r="H2" s="56"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
-        <v>396</v>
+        <v>371</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D3" s="47">
         <v>70</v>
@@ -4419,24 +4661,24 @@
         <v>200</v>
       </c>
       <c r="F3" s="47" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="I3" s="47" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="J3" s="47" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="K3" s="47" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D4" s="47">
         <v>30</v>
@@ -4445,31 +4687,31 @@
         <v>100</v>
       </c>
       <c r="F4" s="47" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F5" s="47" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="47" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E7" s="49" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F7" s="48" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="G7" s="48"/>
       <c r="H7" s="48"/>
@@ -4481,49 +4723,49 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E8" s="47" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="F8" s="47" t="s">
+        <v>309</v>
+      </c>
+      <c r="I8" s="47" t="s">
         <v>313</v>
       </c>
-      <c r="I8" s="47" t="s">
-        <v>317</v>
-      </c>
       <c r="J8" s="47" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E9" s="47" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="I9" s="47" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="J9" s="47" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E10" s="47" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="I10" s="47" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C12" s="49" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D12" s="49" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E12" s="49" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="F12" s="48" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="G12" s="48"/>
       <c r="H12" s="48"/>
@@ -4535,43 +4777,43 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D13" s="47" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="F13" s="47" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="I13" s="47" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D14" s="47" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="I14" s="47" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D15" s="47" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="I15" s="47" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C17" s="49" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D17" s="49" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E17" s="49" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="F17" s="48" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="G17" s="48"/>
       <c r="H17" s="48"/>
@@ -4583,67 +4825,67 @@
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.3">
       <c r="F18" s="47" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="I18" s="47" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="19" spans="3:13" x14ac:dyDescent="0.3">
       <c r="F19" s="47" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="I19" s="47" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="22" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C22" s="52" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D22" s="52" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E22" s="52" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="F22" s="52" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="G22" s="52"/>
       <c r="H22" s="52"/>
       <c r="I22" s="52" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="J22" s="52" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="K22" s="52" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="L22" s="71" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="23" spans="3:13" s="65" customFormat="1" ht="99" x14ac:dyDescent="0.25">
       <c r="C23" s="65" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="D23" s="65" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="E23" s="65" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="F23" s="54" t="str">
         <f>_xlfn.CONCAT(IF(OR(MAX(YI!C21:C23)&gt;$D$3,SUM(YI!C21:C23)&gt;$E$3),$F$3,IF(OR(MAX(YI!C21:C23)&gt;$D$4,SUM(YI!C21:C23)&gt;$E$4),$F$4,$F$5)),D23,$I$3,SUM(YI!C21:C23),$J$3,MAX(YI!C21:C23),$K$3)</f>
-        <v>En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Yí, donde en las últimas 72 horas se acumularon 47.7 mm y con un máximo de 45.7 mm/día.</v>
+        <v>En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Yí, donde en las últimas 72 horas se acumularon 63.8 mm y con un máximo de 63.8 mm/día.</v>
       </c>
       <c r="G23" s="54"/>
       <c r="H23" s="54"/>
       <c r="I23" s="54" t="str">
         <f>_xlfn.CONCAT($F$8,D23,IF(YI!C15=$E$8,$I$8,IF(YI!C15=$E$9,$I$9,$I$10)),$J$8,E23,". ")</f>
-        <v xml:space="preserve">Actualmente, el nivel del río Yí se mantiene constante en la ciudad de Durazno. </v>
+        <v xml:space="preserve">Actualmente, el nivel del río Yí está en ascenso en la ciudad de Durazno. </v>
       </c>
       <c r="J23" s="54" t="str">
         <f>_xlfn.CONCAT(F13,IF(YI!C31&gt;YI!C11,I13, IF(YI!C31=YI!C11,I14, I15)))</f>
@@ -4651,36 +4893,36 @@
       </c>
       <c r="K23" s="54" t="str">
         <f>IF(YI!C13="-","",IF(YI!C31&gt;YI!C13,_xlfn.CONCAT(F18,YI!C13,I18),_xlfn.CONCAT(F19,YI!C13,I19)))</f>
-        <v xml:space="preserve">Existe una alta probabilidad de que el nivel supere al máximo registrado los días anteriores (2.3 metros). </v>
+        <v xml:space="preserve">Existe una alta probabilidad de que el nivel supere al máximo registrado los días anteriores ( metros). </v>
       </c>
       <c r="L23" s="54" t="str">
         <f>+_xlfn.CONCAT(F23," ",I23, " ",J23," ",K23)</f>
-        <v xml:space="preserve">En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Yí, donde en las últimas 72 horas se acumularon 47.7 mm y con un máximo de 45.7 mm/día. Actualmente, el nivel del río Yí se mantiene constante en la ciudad de Durazno.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  Existe una alta probabilidad de que el nivel supere al máximo registrado los días anteriores (2.3 metros). </v>
+        <v xml:space="preserve">En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Yí, donde en las últimas 72 horas se acumularon 63.8 mm y con un máximo de 63.8 mm/día. Actualmente, el nivel del río Yí está en ascenso en la ciudad de Durazno.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  Existe una alta probabilidad de que el nivel supere al máximo registrado los días anteriores ( metros). </v>
       </c>
     </row>
     <row r="24" spans="3:13" ht="82.5" x14ac:dyDescent="0.3">
       <c r="C24" s="53" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="E24" s="53" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="F24" s="55" t="str">
         <f>_xlfn.CONCAT(IF(OR(MAX(CUAREIM!C17:C19)&gt;$D$3,SUM(CUAREIM!C17:C19)&gt;$E$3),$F$3,IF(OR(MAX(CUAREIM!C17:C19)&gt;$D$4,SUM(CUAREIM!C17:C19)&gt;$E$4),$F$4,$F$5)),D24,$I$3,SUM(CUAREIM!C17:C19),$J$3,MAX(CUAREIM!C17:C19),$K$3)</f>
-        <v>En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Cuareim, donde en las últimas 72 horas se acumularon 59.6 mm y con un máximo de 49.5 mm/día.</v>
+        <v>En las últimas horas se registraron bajos acumulados de precipitación en la cuenca del río Cuareim, donde en las últimas 72 horas se acumularon 0 mm y con un máximo de 0 mm/día.</v>
       </c>
       <c r="G24" s="55"/>
       <c r="H24" s="55"/>
       <c r="I24" s="66" t="str">
         <f>_xlfn.CONCAT($F$8,D24,IF(CUAREIM!C16=$E$8,$I$8,IF(CUAREIM!C16=$E$9,$I$9,$I$10)),$J$8,E24,". ")</f>
-        <v xml:space="preserve">Actualmente, el nivel del río Cuareim está en ascenso en la ciudad de Artigas. </v>
+        <v xml:space="preserve">Actualmente, el nivel del río Cuareim se mantiene constante en la ciudad de Artigas. </v>
       </c>
       <c r="J24" s="55" t="str">
         <f>_xlfn.CONCAT(F13,IF(CUAREIM!C27&gt;CUAREIM!C12,I13, IF(CUAREIM!C27=CUAREIM!C12,I14, I15)))</f>
-        <v xml:space="preserve">Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días. </v>
+        <v xml:space="preserve">Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, se prevé que el nivel descienda en los próximos días. </v>
       </c>
       <c r="K24" s="54" t="str">
         <f>IF(CUAREIM!C14="-","",IF(CUAREIM!C27&gt;CUAREIM!C14,_xlfn.CONCAT(F18,CUAREIM!C14,I18),_xlfn.CONCAT(F19,CUAREIM!C14,I19)))</f>
@@ -4688,22 +4930,22 @@
       </c>
       <c r="L24" s="54" t="str">
         <f t="shared" ref="L24:L30" si="0">+_xlfn.CONCAT(F24," ",I24, " ",J24," ",K24)</f>
-        <v xml:space="preserve">En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Cuareim, donde en las últimas 72 horas se acumularon 59.6 mm y con un máximo de 49.5 mm/día. Actualmente, el nivel del río Cuareim está en ascenso en la ciudad de Artigas.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  </v>
+        <v xml:space="preserve">En las últimas horas se registraron bajos acumulados de precipitación en la cuenca del río Cuareim, donde en las últimas 72 horas se acumularon 0 mm y con un máximo de 0 mm/día. Actualmente, el nivel del río Cuareim se mantiene constante en la ciudad de Artigas.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, se prevé que el nivel descienda en los próximos días.  </v>
       </c>
     </row>
     <row r="25" spans="3:13" ht="99" x14ac:dyDescent="0.3">
       <c r="C25" s="53" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E25" s="53" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="F25" s="54" t="str">
         <f>_xlfn.CONCAT(IF(OR(MAX(SANTALUCIA!C27:C29)&gt;$D$3,SUM(SANTALUCIA!C27:C29)&gt;$E$3),$F$3,IF(OR(MAX(SANTALUCIA!C27:C29)&gt;$D$4,SUM(SANTALUCIA!C27:C29)&gt;$E$4),$F$4,$F$5)),D25,$I$3,SUM(SANTALUCIA!C27:C29),$J$3,MAX(SANTALUCIA!C27:C29),$K$3)</f>
-        <v>En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Santa Lucía, donde en las últimas 72 horas se acumularon 105 mm y con un máximo de 35 mm/día.</v>
+        <v>En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Santa Lucía, donde en las últimas 72 horas se acumularon 55.9 mm y con un máximo de 55.9 mm/día.</v>
       </c>
       <c r="G25" s="54"/>
       <c r="H25" s="54"/>
@@ -4717,132 +4959,132 @@
       </c>
       <c r="K25" s="55" t="str">
         <f>IF(SANTALUCIA!C19="-","",IF(SANTALUCIA!C39&gt;SANTALUCIA!C19,_xlfn.CONCAT(F18,SANTALUCIA!C19,I18),_xlfn.CONCAT(F19,SANTALUCIA!C19,I19)))</f>
-        <v>Existe una baja probabilidad de que el nivel supere al máximo registrado los días anteriores (8 metros), pero no se puede descartar en su totalidad.</v>
+        <v xml:space="preserve">Existe una alta probabilidad de que el nivel supere al máximo registrado los días anteriores ( metros). </v>
       </c>
       <c r="L25" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Santa Lucía, donde en las últimas 72 horas se acumularon 105 mm y con un máximo de 35 mm/día. Actualmente, el nivel del río Santa Lucía está en ascenso en la ciudad de Santa Lucía.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  Existe una baja probabilidad de que el nivel supere al máximo registrado los días anteriores (8 metros), pero no se puede descartar en su totalidad.</v>
+        <v xml:space="preserve">En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Santa Lucía, donde en las últimas 72 horas se acumularon 55.9 mm y con un máximo de 55.9 mm/día. Actualmente, el nivel del río Santa Lucía está en ascenso en la ciudad de Santa Lucía.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  Existe una alta probabilidad de que el nivel supere al máximo registrado los días anteriores ( metros). </v>
       </c>
     </row>
     <row r="26" spans="3:13" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C26" s="53" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D26" s="53" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="E26" s="53" t="s">
-        <v>303</v>
-      </c>
-      <c r="F26" s="75" t="str">
+        <v>299</v>
+      </c>
+      <c r="F26" s="76" t="str">
         <f>_xlfn.CONCAT(IF(OR(MAX(URUGUAY!C27:C29)&gt;$D$3,SUM(URUGUAY!C27:C29)&gt;$E$3),$F$3,IF(OR(MAX(URUGUAY!C27:C29)&gt;$D$4,SUM(URUGUAY!C27:C29)&gt;$E$4),$F$4,$F$5)),D26,$I$3,SUM(URUGUAY!C27:C29),$J$3,MAX(URUGUAY!C27:C29),$K$3)</f>
         <v>En las últimas horas se registraron bajos acumulados de precipitación en la cuenca del río Uruguay, donde en las últimas 72 horas se acumularon 0 mm y con un máximo de 0 mm/día.</v>
       </c>
       <c r="I26" s="66" t="str">
         <f>IF(AND(URUGUAY!$C$11=$E$8,URUGUAY!$C$16=$E$8,URUGUAY!$C$21=$E$8,URUGUAY!$C$26=$E$8),_xlfn.CONCAT($F$8,$D$26,$I$8,$J$9," ",E26,", ",E27,", ",E28," y ",Tablas!E29,"."),IF(AND(URUGUAY!$C$11=$E$9,URUGUAY!$C$16=$E$9,URUGUAY!$C$21=$E$9,URUGUAY!$C$26=$E$9),_xlfn.CONCAT($F$8,$D$26,$I$9,$J$9," ",E26,", ",E27,", ",E28," y ",E29,"."),IF(AND(URUGUAY!$C$11=$E$10,URUGUAY!$C$16=$E$10,URUGUAY!$C$21=$E$10,URUGUAY!$C$26=$E$10),_xlfn.CONCAT($F$8,$D$26,$I$10,$J$9," ",E26,", ",E27,", ",E28," y ",E29,"."),_xlfn.CONCAT($F$8,D26,I27,I28,I29))))</f>
-        <v>Actualmente, el nivel del río Uruguay está en ascenso en las ciudades de Bella Unión Paysandú; se mantiene constante en las ciudades de Salto Fray Bentos. está en descenso en la ciudad de .</v>
-      </c>
-      <c r="J26" s="76" t="str">
+        <v>Actualmente, el nivel del río Uruguay está en ascenso en la ciudad de ; se mantiene constante en las ciudades de Bella Unión Salto Paysandú; está en descenso en la ciudad de  Fray Bentos.</v>
+      </c>
+      <c r="J26" s="77" t="str">
         <f>_xlfn.CONCAT(F13,IF(AND(URUGUAY!C31&gt;URUGUAY!C7, URUGUAY!C33&gt;URUGUAY!C12, URUGUAY!C35&gt;URUGUAY!C17, URUGUAY!C37&gt;URUGUAY!C22),I13, IF(AND(URUGUAY!C31=URUGUAY!C7, URUGUAY!C33=URUGUAY!C12, URUGUAY!C35=URUGUAY!C17, URUGUAY!C37=URUGUAY!C22),I14, I15)))</f>
-        <v xml:space="preserve">Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días. </v>
-      </c>
-      <c r="K26" s="76" t="str">
+        <v xml:space="preserve">Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, se prevé que el nivel descienda en los próximos días. </v>
+      </c>
+      <c r="K26" s="77" t="str">
         <f>IF(AND(URUGUAY!C9="-", URUGUAY!C14="-", URUGUAY!C19="-", URUGUAY!C24="-"),"",IF(OR(URUGUAY!C31&gt;URUGUAY!C9, URUGUAY!C33&gt;URUGUAY!C14, URUGUAY!C35&gt;URUGUAY!C19,URUGUAY!C37&gt;URUGUAY!C24),_xlfn.CONCAT(F18,IF(URUGUAY!C9&lt;&gt;"-",_xlfn.CONCAT(URUGUAY!C9,"m en ",E26," "),""), IF(URUGUAY!C14&lt;&gt;"-",_xlfn.CONCAT(URUGUAY!C14, "m en ",E27," "),""),IF(URUGUAY!C19&lt;&gt;"-",_xlfn.CONCAT(URUGUAY!C19,"m en ",E28," "),""),IF(URUGUAY!C24&lt;&gt;"-",_xlfn.CONCAT(URUGUAY!C24,"m en ",E29),""),")."),_xlfn.CONCAT(F19,IF(URUGUAY!C9&lt;&gt;"-",_xlfn.CONCAT(URUGUAY!C9,"m en ",E26," "),""), IF(URUGUAY!C14&lt;&gt;"-",_xlfn.CONCAT(URUGUAY!C14, "m en ",E27," "),""),IF(URUGUAY!C19&lt;&gt;"-",_xlfn.CONCAT(URUGUAY!C19,"m en ",E28," "),""),IF(URUGUAY!C24&lt;&gt;"-",_xlfn.CONCAT(URUGUAY!C24,"m en ",E29),""),", pero no se puede descartar en su totalidad.")))</f>
-        <v>Existe una alta probabilidad de que el nivel supere al máximo registrado los días anteriores (5m en Paysandú ).</v>
-      </c>
-      <c r="L26" s="76" t="str">
+        <v>Existe una baja probabilidad de que el nivel supere al máximo registrado los días anteriores (7.89m en Paysandú , pero no se puede descartar en su totalidad.</v>
+      </c>
+      <c r="L26" s="77" t="str">
         <f t="shared" si="0"/>
-        <v>En las últimas horas se registraron bajos acumulados de precipitación en la cuenca del río Uruguay, donde en las últimas 72 horas se acumularon 0 mm y con un máximo de 0 mm/día. Actualmente, el nivel del río Uruguay está en ascenso en las ciudades de Bella Unión Paysandú; se mantiene constante en las ciudades de Salto Fray Bentos. está en descenso en la ciudad de . Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  Existe una alta probabilidad de que el nivel supere al máximo registrado los días anteriores (5m en Paysandú ).</v>
-      </c>
-    </row>
-    <row r="27" spans="3:13" ht="33" x14ac:dyDescent="0.3">
+        <v>En las últimas horas se registraron bajos acumulados de precipitación en la cuenca del río Uruguay, donde en las últimas 72 horas se acumularon 0 mm y con un máximo de 0 mm/día. Actualmente, el nivel del río Uruguay está en ascenso en la ciudad de ; se mantiene constante en las ciudades de Bella Unión Salto Paysandú; está en descenso en la ciudad de  Fray Bentos. Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, se prevé que el nivel descienda en los próximos días.  Existe una baja probabilidad de que el nivel supere al máximo registrado los días anteriores (7.89m en Paysandú , pero no se puede descartar en su totalidad.</v>
+      </c>
+    </row>
+    <row r="27" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C27" s="53"/>
       <c r="D27" s="53"/>
       <c r="E27" s="53" t="s">
-        <v>304</v>
-      </c>
-      <c r="F27" s="75"/>
+        <v>300</v>
+      </c>
+      <c r="F27" s="76"/>
       <c r="G27" s="60">
         <f>SUM(URUGUAY!$C$11=Tablas!E8, URUGUAY!$C$16=Tablas!E8,URUGUAY!$C$21=Tablas!E8,URUGUAY!$C$26=Tablas!E8)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H27" s="61" t="str">
         <f>_xlfn.CONCAT(IF(URUGUAY!$C$11=Tablas!E8,_xlfn.CONCAT(" ",$E$26,),""),IF(URUGUAY!$C$16=Tablas!E8,_xlfn.CONCAT(" ",$E$27),""),IF(URUGUAY!$C$21=Tablas!E8,_xlfn.CONCAT(" ",$E$28),""),IF(URUGUAY!$C$26=Tablas!E8,_xlfn.CONCAT(" ",$E$29),""))</f>
-        <v xml:space="preserve"> Bella Unión Paysandú</v>
+        <v/>
       </c>
       <c r="I27" s="67" t="str">
         <f>_xlfn.CONCAT(I8,IF(G27&gt;1,$J$9,$J$8),H27, IF(G27=4,".", ";"))</f>
-        <v xml:space="preserve"> está en ascenso en las ciudades de Bella Unión Paysandú;</v>
-      </c>
-      <c r="J27" s="76"/>
-      <c r="K27" s="76"/>
-      <c r="L27" s="76"/>
+        <v xml:space="preserve"> está en ascenso en la ciudad de ;</v>
+      </c>
+      <c r="J27" s="77"/>
+      <c r="K27" s="77"/>
+      <c r="L27" s="77"/>
     </row>
     <row r="28" spans="3:13" ht="33" x14ac:dyDescent="0.3">
       <c r="C28" s="53"/>
       <c r="D28" s="53"/>
       <c r="E28" s="53" t="s">
-        <v>305</v>
-      </c>
-      <c r="F28" s="75"/>
+        <v>301</v>
+      </c>
+      <c r="F28" s="76"/>
       <c r="G28" s="60">
         <f>SUM(URUGUAY!$C$11=Tablas!E9, URUGUAY!$C$16=Tablas!E9,URUGUAY!$C$21=Tablas!E9,URUGUAY!$C$26=Tablas!E9)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H28" s="61" t="str">
         <f>_xlfn.CONCAT(IF(URUGUAY!$C$11=Tablas!E9,_xlfn.CONCAT(" ",$E$26),""),IF(URUGUAY!$C$16=Tablas!E9,_xlfn.CONCAT(" ",$E$27),""),IF(URUGUAY!$C$21=Tablas!E9,_xlfn.CONCAT(" ",$E$28),""),IF(URUGUAY!$C$26=Tablas!E9,_xlfn.CONCAT(" ",$E$29),""))</f>
-        <v xml:space="preserve"> Salto Fray Bentos</v>
+        <v xml:space="preserve"> Bella Unión Salto Paysandú</v>
       </c>
       <c r="I28" s="67" t="str">
         <f>_xlfn.CONCAT(I9,IF(G28&gt;1,$J$9,$J$8),H28, IF((G27+G28)=4,".", ";"))</f>
-        <v xml:space="preserve"> se mantiene constante en las ciudades de Salto Fray Bentos.</v>
-      </c>
-      <c r="J28" s="76"/>
-      <c r="K28" s="76"/>
-      <c r="L28" s="76"/>
+        <v xml:space="preserve"> se mantiene constante en las ciudades de Bella Unión Salto Paysandú;</v>
+      </c>
+      <c r="J28" s="77"/>
+      <c r="K28" s="77"/>
+      <c r="L28" s="77"/>
     </row>
     <row r="29" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C29" s="53"/>
       <c r="D29" s="53"/>
       <c r="E29" s="53" t="s">
-        <v>306</v>
-      </c>
-      <c r="F29" s="75"/>
+        <v>302</v>
+      </c>
+      <c r="F29" s="76"/>
       <c r="G29" s="60">
         <f>SUM(URUGUAY!$C$11=Tablas!E10, URUGUAY!$C$16=Tablas!E10,URUGUAY!$C$21=Tablas!E10,URUGUAY!$C$26=Tablas!E10)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" s="61" t="str">
         <f>_xlfn.CONCAT(IF(URUGUAY!$C$11=Tablas!E10,_xlfn.CONCAT(" ",$E$26),""),IF(URUGUAY!$C$16=Tablas!E10,_xlfn.CONCAT(" ",$E$27),""),IF(URUGUAY!$C$21=Tablas!E10,_xlfn.CONCAT(" ",$E$28),""),IF(URUGUAY!$C$26=Tablas!E10,_xlfn.CONCAT(" ",$E$29),""))</f>
-        <v/>
+        <v xml:space="preserve"> Fray Bentos</v>
       </c>
       <c r="I29" s="67" t="str">
         <f>_xlfn.CONCAT(I10,IF(G29&gt;1,$J$9,$J$8),H29, ".")</f>
-        <v xml:space="preserve"> está en descenso en la ciudad de .</v>
-      </c>
-      <c r="J29" s="76"/>
-      <c r="K29" s="76"/>
-      <c r="L29" s="76"/>
+        <v xml:space="preserve"> está en descenso en la ciudad de  Fray Bentos.</v>
+      </c>
+      <c r="J29" s="77"/>
+      <c r="K29" s="77"/>
+      <c r="L29" s="77"/>
     </row>
     <row r="30" spans="3:13" ht="82.5" x14ac:dyDescent="0.3">
       <c r="C30" s="53" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D30" s="53" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="E30" s="53" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="F30" s="54" t="str">
         <f>_xlfn.CONCAT(IF(OR(MAX(NEGRO!C12:C14)&gt;$D$3,SUM(NEGRO!C12:C14)&gt;$E$3),$F$3,IF(OR(MAX(NEGRO!C12:C14)&gt;$D$4,SUM(NEGRO!C12:C14)&gt;$E$4),$F$4,$F$5)),D30,$I$3,SUM(NEGRO!C12:C14),$J$3,MAX(NEGRO!C12:C14),$K$3)</f>
-        <v>En las últimas horas se registraron importantes acumulados de precipitación en la cuenca del Río Negro, donde en las últimas 72 horas se acumularon 210 mm y con un máximo de 70 mm/día.</v>
+        <v>En las últimas horas se registraron bajos acumulados de precipitación en la cuenca del Río Negro, donde en las últimas 72 horas se acumularon 0 mm y con un máximo de 0 mm/día.</v>
       </c>
       <c r="G30" s="54"/>
       <c r="H30" s="54"/>
       <c r="I30" s="66" t="str">
         <f>_xlfn.CONCAT($F$8,D30,IF(NEGRO!C11=$E$8,$I$8,IF(NEGRO!C11=$E$9,$I$9,$I$10)),$J$8,E30,". ")</f>
-        <v xml:space="preserve">Actualmente, el nivel del Río Negro está en ascenso en la ciudad de Mercedes. </v>
+        <v xml:space="preserve">Actualmente, el nivel del Río Negro se mantiene constante en la ciudad de Mercedes. </v>
       </c>
       <c r="J30" s="55" t="str">
         <f>_xlfn.CONCAT(F13,IF(NEGRO!C19&gt;NEGRO!C7,I13, IF(NEGRO!C19=NEGRO!C7,I14, I15)))</f>
@@ -4854,7 +5096,7 @@
       </c>
       <c r="L30" s="54" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">En las últimas horas se registraron importantes acumulados de precipitación en la cuenca del Río Negro, donde en las últimas 72 horas se acumularon 210 mm y con un máximo de 70 mm/día. Actualmente, el nivel del Río Negro está en ascenso en la ciudad de Mercedes.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  </v>
+        <v xml:space="preserve">En las últimas horas se registraron bajos acumulados de precipitación en la cuenca del Río Negro, donde en las últimas 72 horas se acumularon 0 mm y con un máximo de 0 mm/día. Actualmente, el nivel del Río Negro se mantiene constante en la ciudad de Mercedes.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  </v>
       </c>
     </row>
   </sheetData>
@@ -4873,7 +5115,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47D3EC66-79F8-4D4E-901B-5FC0A35308DF}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -4891,16 +5133,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B1" s="59" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C1" s="62" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="D1" s="62" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4908,13 +5150,13 @@
         <v>45224</v>
       </c>
       <c r="B2" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C2" s="63" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="D2" s="63" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -4922,10 +5164,10 @@
         <v>45224</v>
       </c>
       <c r="B3" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C3" s="63" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -4933,13 +5175,13 @@
         <v>45224</v>
       </c>
       <c r="B4" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C4" s="63" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="D4" s="63" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4947,10 +5189,10 @@
         <v>45224</v>
       </c>
       <c r="B5" t="s">
+        <v>353</v>
+      </c>
+      <c r="C5" s="63" t="s">
         <v>357</v>
-      </c>
-      <c r="C5" s="63" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4958,10 +5200,10 @@
         <v>45224</v>
       </c>
       <c r="B6" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D6" s="64" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4969,13 +5211,13 @@
         <v>45224</v>
       </c>
       <c r="B7" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C7" s="63" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D7" s="63" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Design a flood service for San Jose river basin
</commit_message>
<xml_diff>
--- a/automatic docx/database_report.xlsx
+++ b/automatic docx/database_report.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Python Scripts\automatic docx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221577AB-5914-45F0-B1B9-6FC7266232AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590E388A-039E-46E8-BDAF-E46D2BA92606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{83108E16-E9D6-4CCB-B5BE-A67101359CD3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{83108E16-E9D6-4CCB-B5BE-A67101359CD3}"/>
   </bookViews>
   <sheets>
     <sheet name="INICIO" sheetId="1" r:id="rId1"/>
     <sheet name="YI" sheetId="2" r:id="rId2"/>
     <sheet name="CUAREIM" sheetId="4" r:id="rId3"/>
     <sheet name="SANTALUCIA" sheetId="5" r:id="rId4"/>
-    <sheet name="URUGUAY" sheetId="7" r:id="rId5"/>
-    <sheet name="NEGRO" sheetId="6" r:id="rId6"/>
-    <sheet name="OLIMAR" sheetId="10" r:id="rId7"/>
-    <sheet name="Tablas" sheetId="8" r:id="rId8"/>
-    <sheet name="log" sheetId="9" r:id="rId9"/>
+    <sheet name="SANJOSE" sheetId="11" r:id="rId5"/>
+    <sheet name="URUGUAY" sheetId="7" r:id="rId6"/>
+    <sheet name="NEGRO" sheetId="6" r:id="rId7"/>
+    <sheet name="OLIMAR" sheetId="10" r:id="rId8"/>
+    <sheet name="Tablas" sheetId="8" r:id="rId9"/>
+    <sheet name="log" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="443">
   <si>
     <t>fecha_emision</t>
   </si>
@@ -1305,6 +1306,72 @@
   </si>
   <si>
     <t>30 Octubre</t>
+  </si>
+  <si>
+    <t>Pronostico hidrologico en San Ramón</t>
+  </si>
+  <si>
+    <t>fecha ocurrencia nivel máximo en San Ramón</t>
+  </si>
+  <si>
+    <t>pronos_ramon</t>
+  </si>
+  <si>
+    <t>fecha_ramon</t>
+  </si>
+  <si>
+    <t>Pronóstico hidrológico en Canelones</t>
+  </si>
+  <si>
+    <t>fecha de ocurrencia nivel máximo en Canelones</t>
+  </si>
+  <si>
+    <t>pronos_canelones</t>
+  </si>
+  <si>
+    <t>fecha_canelones</t>
+  </si>
+  <si>
+    <t>pobs_24_jose</t>
+  </si>
+  <si>
+    <t>pobs_48_jose</t>
+  </si>
+  <si>
+    <t>pobs_72_jose</t>
+  </si>
+  <si>
+    <t>psim_24_jose</t>
+  </si>
+  <si>
+    <t>psim_48_jose</t>
+  </si>
+  <si>
+    <t>psim_72_jose</t>
+  </si>
+  <si>
+    <t>diagnostico_jose</t>
+  </si>
+  <si>
+    <t>recomendacion_jose</t>
+  </si>
+  <si>
+    <t>Superior a 7 metros</t>
+  </si>
+  <si>
+    <t>Entre 25 al 30 octubre</t>
+  </si>
+  <si>
+    <t>Menor a 2.0 m</t>
+  </si>
+  <si>
+    <t>Entre 29 al 30 mayo</t>
+  </si>
+  <si>
+    <t>10.8 m</t>
+  </si>
+  <si>
+    <t>31 mayo</t>
   </si>
 </sst>
 </file>
@@ -2262,6 +2329,117 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47D3EC66-79F8-4D4E-901B-5FC0A35308DF}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="94.140625" style="63" customWidth="1"/>
+    <col min="4" max="4" width="78.5703125" style="63" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="59" t="s">
+        <v>350</v>
+      </c>
+      <c r="B1" s="59" t="s">
+        <v>351</v>
+      </c>
+      <c r="C1" s="62" t="s">
+        <v>352</v>
+      </c>
+      <c r="D1" s="62" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="58">
+        <v>45224</v>
+      </c>
+      <c r="B2" t="s">
+        <v>353</v>
+      </c>
+      <c r="C2" s="63" t="s">
+        <v>354</v>
+      </c>
+      <c r="D2" s="63" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="58">
+        <v>45224</v>
+      </c>
+      <c r="B3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C3" s="63" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="58">
+        <v>45224</v>
+      </c>
+      <c r="B4" t="s">
+        <v>353</v>
+      </c>
+      <c r="C4" s="63" t="s">
+        <v>356</v>
+      </c>
+      <c r="D4" s="63" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="58">
+        <v>45224</v>
+      </c>
+      <c r="B5" t="s">
+        <v>353</v>
+      </c>
+      <c r="C5" s="63" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="58">
+        <v>45224</v>
+      </c>
+      <c r="B6" t="s">
+        <v>353</v>
+      </c>
+      <c r="D6" s="64" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="58">
+        <v>45224</v>
+      </c>
+      <c r="B7" t="s">
+        <v>353</v>
+      </c>
+      <c r="C7" s="63" t="s">
+        <v>368</v>
+      </c>
+      <c r="D7" s="63" t="s">
+        <v>369</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88EDC221-CFDF-4572-98F1-7407159CEFB9}">
   <dimension ref="A1:C36"/>
@@ -3103,10 +3281,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE02CEB0-09AB-4ABD-86C9-DCBCC2E88044}">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -3238,43 +3416,45 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="C12" s="8"/>
+        <v>167</v>
+      </c>
+      <c r="C12" s="8">
+        <v>7.91</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="C13" s="6"/>
+        <v>168</v>
+      </c>
+      <c r="C13" s="6">
+        <v>7.86</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>255</v>
-      </c>
+        <v>337</v>
+      </c>
+      <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
         <v>44</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="C15" s="32">
         <f>IF((C12-C13)&gt;=0,ROUND((C12-C13)*100,0),"")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3282,41 +3462,37 @@
         <v>45</v>
       </c>
       <c r="B16" s="38" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="C16" s="39" t="str">
         <f>IF(C15=0,"Permanece",IF(C15="","Baja","Sube"))</f>
-        <v>Permanece</v>
+        <v>Sube</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="C17" s="8">
-        <v>7.91</v>
-      </c>
+      <c r="A17" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C17" s="6"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="C18" s="6">
-        <v>7.86</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="C18" s="6"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C19" s="6"/>
     </row>
@@ -3325,11 +3501,11 @@
         <v>44</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>169</v>
+        <v>133</v>
       </c>
       <c r="C20" s="32">
-        <f>IF((C17-C18)&gt;=0,ROUND((C17-C18)*100,0),"")</f>
-        <v>5</v>
+        <f>IFERROR(ROUND(ABS(C17-C18)*100,0),"-")</f>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3337,251 +3513,230 @@
         <v>45</v>
       </c>
       <c r="B21" s="38" t="s">
-        <v>170</v>
+        <v>134</v>
       </c>
       <c r="C21" s="39" t="str">
-        <f>IF(C20=0,"Permanece",IF(C20="","Baja","Sube"))</f>
-        <v>Sube</v>
+        <f>IFERROR(IF(C20=0,"Permanece",IF(SIGN(C20)=1,"Sube","Baja")),"-")</f>
+        <v>Permanece</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="27" t="s">
-        <v>141</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C22" s="6"/>
+      <c r="A22" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
-        <v>142</v>
+        <v>53</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C23" s="6"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="27" t="s">
-        <v>338</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>339</v>
-      </c>
-      <c r="C24" s="6"/>
+        <v>114</v>
+      </c>
+      <c r="C23" s="6">
+        <v>55.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="C25" s="32">
-        <f>IFERROR(ROUND(ABS(C22-C23)*100,0),"-")</f>
+      <c r="A25" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C25" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="B26" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="C26" s="39" t="str">
-        <f>IFERROR(IF(C25=0,"Permanece",IF(SIGN(C25)=1,"Sube","Baja")),"-")</f>
-        <v>Permanece</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="C27" s="8">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" s="6">
         <v>0</v>
       </c>
     </row>
+    <row r="27" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" s="10">
+        <v>0</v>
+      </c>
+    </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C28" s="6">
-        <v>55.9</v>
+      <c r="A28" s="28" t="s">
+        <v>421</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="29" t="s">
-        <v>54</v>
+        <v>422</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="C29" s="10">
-        <v>0</v>
+        <v>424</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C30" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C31" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="C32" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="28" t="s">
+      <c r="A30" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B30" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="C33" s="11"/>
-    </row>
-    <row r="34" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="29" t="s">
+      <c r="C30" s="11" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B31" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="C34" s="12"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="28" t="s">
+      <c r="C31" s="12" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B32" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="C35" s="11"/>
-    </row>
-    <row r="36" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="29" t="s">
+      <c r="C32" s="11" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="29" t="s">
         <v>152</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B33" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="C36" s="12"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="27" t="s">
-        <v>159</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="C37" s="11" t="s">
+      <c r="C33" s="12" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="27" t="s">
+        <v>425</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="C34" s="11" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="27" t="s">
-        <v>160</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="C38" s="12" t="s">
+    <row r="35" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="27" t="s">
+        <v>426</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="C35" s="12" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="28" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B36" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C36" s="11" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="29" t="s">
+    <row r="37" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="29" t="s">
         <v>140</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B37" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C37" s="12" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="28" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B38" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C38" s="11" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="29" t="s">
+    <row r="39" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B39" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="C39" s="12" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="28" t="s">
+    <row r="40" spans="1:3" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B40" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="C40" s="13" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="30" t="s">
+    <row r="41" spans="1:3" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="B44" s="14" t="s">
+      <c r="B41" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="C44" s="15" t="s">
+      <c r="C41" s="15" t="s">
         <v>394</v>
       </c>
     </row>
@@ -3594,13 +3749,13 @@
           <x14:formula1>
             <xm:f>Tablas!$A$2:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>C44</xm:sqref>
+          <xm:sqref>C41</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{3C04FF7D-FB36-4650-A00C-7C8C9E025181}">
           <x14:formula1>
             <xm:f>Tablas!$L$25</xm:f>
           </x14:formula1>
-          <xm:sqref>C43</xm:sqref>
+          <xm:sqref>C40</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3609,6 +3764,223 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5F464D-9489-4499-83A6-0FFC57B0DDBD}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="52.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="48.28515625" style="5" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C3" s="6">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
+        <v>335</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>157</v>
+      </c>
+      <c r="C5" s="32">
+        <f>IF((C2-C3)&gt;=0,ROUND((C2-C3)*100,0),"")</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="C6" s="39" t="str">
+        <f>IF(C5=0,"Permanece",IF(C5="","Baja","Sube"))</f>
+        <v>Sube</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="C7" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="C8" s="6">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>431</v>
+      </c>
+      <c r="C9" s="10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="C10" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="C11" s="6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>434</v>
+      </c>
+      <c r="C12" s="10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>436</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>394</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{CB07A3A1-E957-443D-BA3B-C8739971E1B2}">
+          <x14:formula1>
+            <xm:f>Tablas!$L$25</xm:f>
+          </x14:formula1>
+          <xm:sqref>C15</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{4F9037B6-004D-4786-812A-241DE34D38BA}">
+          <x14:formula1>
+            <xm:f>Tablas!$A$2:$A$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>C16</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2155F922-1445-4239-A643-A9F5E09853DC}">
   <dimension ref="A1:D40"/>
   <sheetViews>
@@ -4086,7 +4458,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7698158D-7CF5-4621-99AA-4EF5CEB60D57}">
   <dimension ref="A1:C22"/>
   <sheetViews>
@@ -4367,11 +4739,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F4874F4-C602-4D36-9B06-CCCD4B9EE49C}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
@@ -4586,7 +4958,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F783B566-6E24-4EBC-9E3F-D2E3A05600BD}">
   <dimension ref="A1:M30"/>
   <sheetViews>
@@ -4944,21 +5316,21 @@
         <v>286</v>
       </c>
       <c r="F25" s="54" t="str">
-        <f>_xlfn.CONCAT(IF(OR(MAX(SANTALUCIA!C27:C29)&gt;$D$3,SUM(SANTALUCIA!C27:C29)&gt;$E$3),$F$3,IF(OR(MAX(SANTALUCIA!C27:C29)&gt;$D$4,SUM(SANTALUCIA!C27:C29)&gt;$E$4),$F$4,$F$5)),D25,$I$3,SUM(SANTALUCIA!C27:C29),$J$3,MAX(SANTALUCIA!C27:C29),$K$3)</f>
+        <f>_xlfn.CONCAT(IF(OR(MAX(SANTALUCIA!C22:C24)&gt;$D$3,SUM(SANTALUCIA!C22:C24)&gt;$E$3),$F$3,IF(OR(MAX(SANTALUCIA!C22:C24)&gt;$D$4,SUM(SANTALUCIA!C22:C24)&gt;$E$4),$F$4,$F$5)),D25,$I$3,SUM(SANTALUCIA!C22:C24),$J$3,MAX(SANTALUCIA!C22:C24),$K$3)</f>
         <v>En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Santa Lucía, donde en las últimas 72 horas se acumularon 55.9 mm y con un máximo de 55.9 mm/día.</v>
       </c>
       <c r="G25" s="54"/>
       <c r="H25" s="54"/>
       <c r="I25" s="66" t="str">
-        <f>_xlfn.CONCAT($F$8,D25,IF(SANTALUCIA!C21=$E$8,$I$8,IF(SANTALUCIA!C21=$E$9,$I$9,$I$10)),$J$8,E25,". ")</f>
+        <f>_xlfn.CONCAT($F$8,D25,IF(SANTALUCIA!C16=$E$8,$I$8,IF(SANTALUCIA!C16=$E$9,$I$9,$I$10)),$J$8,E25,". ")</f>
         <v xml:space="preserve">Actualmente, el nivel del río Santa Lucía está en ascenso en la ciudad de Santa Lucía. </v>
       </c>
       <c r="J25" s="55" t="str">
-        <f>_xlfn.CONCAT(F13,IF(SANTALUCIA!C39&gt;SANTALUCIA!C17,I13, IF(SANTALUCIA!C39=SANTALUCIA!C17,I14, I15)))</f>
+        <f>_xlfn.CONCAT(F13,IF(SANTALUCIA!C36&gt;SANTALUCIA!C12,I13, IF(SANTALUCIA!C36=SANTALUCIA!C12,I14, I15)))</f>
         <v xml:space="preserve">Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días. </v>
       </c>
       <c r="K25" s="55" t="str">
-        <f>IF(SANTALUCIA!C19="-","",IF(SANTALUCIA!C39&gt;SANTALUCIA!C19,_xlfn.CONCAT(F18,SANTALUCIA!C19,I18),_xlfn.CONCAT(F19,SANTALUCIA!C19,I19)))</f>
+        <f>IF(SANTALUCIA!C14="-","",IF(SANTALUCIA!C36&gt;SANTALUCIA!C14,_xlfn.CONCAT(F18,SANTALUCIA!C14,I18),_xlfn.CONCAT(F19,SANTALUCIA!C14,I19)))</f>
         <v xml:space="preserve">Existe una alta probabilidad de que el nivel supere al máximo registrado los días anteriores ( metros). </v>
       </c>
       <c r="L25" s="54" t="str">
@@ -5113,115 +5485,4 @@
     <ignoredError sqref="F23:F25" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47D3EC66-79F8-4D4E-901B-5FC0A35308DF}">
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="94.140625" style="63" customWidth="1"/>
-    <col min="4" max="4" width="78.5703125" style="63" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
-        <v>350</v>
-      </c>
-      <c r="B1" s="59" t="s">
-        <v>351</v>
-      </c>
-      <c r="C1" s="62" t="s">
-        <v>352</v>
-      </c>
-      <c r="D1" s="62" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="58">
-        <v>45224</v>
-      </c>
-      <c r="B2" t="s">
-        <v>353</v>
-      </c>
-      <c r="C2" s="63" t="s">
-        <v>354</v>
-      </c>
-      <c r="D2" s="63" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="58">
-        <v>45224</v>
-      </c>
-      <c r="B3" t="s">
-        <v>353</v>
-      </c>
-      <c r="C3" s="63" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="58">
-        <v>45224</v>
-      </c>
-      <c r="B4" t="s">
-        <v>353</v>
-      </c>
-      <c r="C4" s="63" t="s">
-        <v>356</v>
-      </c>
-      <c r="D4" s="63" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="58">
-        <v>45224</v>
-      </c>
-      <c r="B5" t="s">
-        <v>353</v>
-      </c>
-      <c r="C5" s="63" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="58">
-        <v>45224</v>
-      </c>
-      <c r="B6" t="s">
-        <v>353</v>
-      </c>
-      <c r="D6" s="64" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="58">
-        <v>45224</v>
-      </c>
-      <c r="B7" t="s">
-        <v>353</v>
-      </c>
-      <c r="C7" s="63" t="s">
-        <v>368</v>
-      </c>
-      <c r="D7" s="63" t="s">
-        <v>369</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
update new logo in the master doc and GIS maps
</commit_message>
<xml_diff>
--- a/automatic docx/database_report.xlsx
+++ b/automatic docx/database_report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Python Scripts\automatic docx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Sala_Situacion_Dinagua\automatic docx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590E388A-039E-46E8-BDAF-E46D2BA92606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9128F851-17F4-4471-AF17-4E0511066936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{83108E16-E9D6-4CCB-B5BE-A67101359CD3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{83108E16-E9D6-4CCB-B5BE-A67101359CD3}"/>
   </bookViews>
   <sheets>
     <sheet name="INICIO" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="441">
   <si>
     <t>fecha_emision</t>
   </si>
@@ -1179,18 +1179,6 @@
     <t>Estar preparados ante la posibilidad de inundaciones que afecten a zona de vivienda.</t>
   </si>
   <si>
-    <t>Menor a 8.5 m</t>
-  </si>
-  <si>
-    <t>Entre 29 - 30 mayo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29 mayo </t>
-  </si>
-  <si>
-    <t>29 - 30 mayo</t>
-  </si>
-  <si>
     <t>10 mm en la parte alta de la cuenca</t>
   </si>
   <si>
@@ -1209,9 +1197,6 @@
     <t xml:space="preserve">Estar atentos a los incrementos de nivel del río Negro en el tramo Represa Constitución y Mercedes. </t>
   </si>
   <si>
-    <t>Se mantienen los incrementos de nivel en los ríos Yí y Santa Lucía.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Actualmente se encuentra en tránsito una crecida del río Yí en el tramo Polanco del Yí y Durazno. En Sarandí Yí se registró el dia de ayer un nivel máximo de 5.44 m y actualmente se encuentra en descenso. En Polanco del Yí se encuentra en ascenso el nivel del río en una cota de 8.39 m (3 cm/h). En Durazno puente viejo se tiene un nivel de 9.14 m (Puente Ruta 5) y 8.05 m (en Puente Viejo). Estos niveles estan en ascenso y aun por debajo de la cota de seguridad (8.2 m en Durazno Puente Viejo). En base a estas condiciones se espera que se mantenga en ascenso el nivel del río Yí y superando la cota de seguridad en el transcurso del día. Actualmente el nivel máximo pronosticado para Durazno seria entre 8.2 a 8.6 metros en Durazno puente viejo para 02 o 03 de mayo. </t>
   </si>
   <si>
@@ -1221,15 +1206,6 @@
     <t>Menor a 4.0 m</t>
   </si>
   <si>
-    <t>Menor a 5.50 m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Se encuentra en ascenso el nivel del río Santa Lucia en Ruta 11 (7.61 m), Aguas corrientes (5.17 m). OSE reporta que el nivel del embalse Paso severino es de 38.94 m. De acuerdo a la información brindada el día de ayer, se espera que en el transcurso de este día y mañana se tenga el nivel máximo del río Santa Lucia en Ruta 11, llegando a un nivel menor a 8.5 m y por debajo levemente de la cota de seguridad (9.36 m). </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estar atentos a los incrementos de nivel que está experimentando el río Santa Lucia. </t>
-  </si>
-  <si>
     <t>entre 12,800 y 13,800</t>
   </si>
   <si>
@@ -1356,22 +1332,40 @@
     <t>recomendacion_jose</t>
   </si>
   <si>
-    <t>Superior a 7 metros</t>
-  </si>
-  <si>
-    <t>Entre 25 al 30 octubre</t>
-  </si>
-  <si>
     <t>Menor a 2.0 m</t>
   </si>
   <si>
-    <t>Entre 29 al 30 mayo</t>
-  </si>
-  <si>
-    <t>10.8 m</t>
-  </si>
-  <si>
-    <t>31 mayo</t>
+    <t>Alrededor de 7 metros</t>
+  </si>
+  <si>
+    <t>Entre 04 y 05 de marzo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estar preparados a posibilidad de inundaciones y afectación a vivienda en San José. </t>
+  </si>
+  <si>
+    <t>Entre el 05 y 06 marzo</t>
+  </si>
+  <si>
+    <t>05 de marzo</t>
+  </si>
+  <si>
+    <t>Menor a 4.5 m</t>
+  </si>
+  <si>
+    <t>Entre el 07 y 08 marzo</t>
+  </si>
+  <si>
+    <t>En la ultima semana se registraron 137 mm y 104.5 mm acumulado de lluvia en las subcuencas de los ríos Santa Lucia Chico y Grande, respectivamente. Se espera incrementos de nivel del río Santa Lucia Chico y el Santa Lucia desde el tramo de Paso Pache hasta Aguas Corrientes en los próximos días, dado que el mayor aporte vendría de ese lado de la cuenca (Santa Lucia Chico) que del río Santa Lucia Grande. Según datos que nos pasa la OSE, antes del evento Paso Severino estaba a un 84,4% de capacidad de almacenaje y buena parte de la crecida ayudaría a volver a llenar el embalse (actualmente está aumentando a 93,4% de volumen almacenado)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estar atentos al incremento del nivel del río Santa Lucia Grande y Chico. </t>
+  </si>
+  <si>
+    <t>Se registran incrementos significativos de nivel en los ríos San José, Santa Lucia Chico y los que drenan hasta el Río de la Plata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En la ultima semana se han registrado 127.5 mm de lluvia en la cuenca del río San Jose, registrandose entre las 7 hrs del 03-Marzo hasta las 7 hrs 04-Marzo un acumulado de 64 mm en promedio. Actualmente CECOED San José reporta un incremento del nivel del río San José cercano a los 7.3 metros, lo cual estaria superando la cota de seguridad (7.4 m) definido para la ciudad. Se debe estar atentos y estar preparados dado que el nivel máximo aun no ha llegado. </t>
   </si>
 </sst>
 </file>
@@ -2237,7 +2231,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="41">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2249,7 +2243,7 @@
       </c>
       <c r="C3" s="42">
         <f ca="1">TODAY()</f>
-        <v>45593</v>
+        <v>45720</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -2261,7 +2255,7 @@
       </c>
       <c r="C4" s="43">
         <f ca="1">$C$3-1</f>
-        <v>45592</v>
+        <v>45719</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2273,7 +2267,7 @@
       </c>
       <c r="C5" s="42">
         <f ca="1">$C$3-2</f>
-        <v>45591</v>
+        <v>45718</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -2285,7 +2279,7 @@
       </c>
       <c r="C6" s="43">
         <f ca="1">$C$3+1</f>
-        <v>45594</v>
+        <v>45721</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -2297,7 +2291,7 @@
       </c>
       <c r="C7" s="44">
         <f ca="1">$C$3+2</f>
-        <v>45595</v>
+        <v>45722</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2309,7 +2303,7 @@
       </c>
       <c r="C8" s="42">
         <f ca="1">$C$3+3</f>
-        <v>45596</v>
+        <v>45723</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2320,7 +2314,7 @@
         <v>172</v>
       </c>
       <c r="C9" s="45" t="s">
-        <v>388</v>
+        <v>439</v>
       </c>
     </row>
   </sheetData>
@@ -2839,7 +2833,7 @@
         <v>39</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3203,7 +3197,7 @@
         <v>81</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3283,8 +3277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE02CEB0-09AB-4ABD-86C9-DCBCC2E88044}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -3314,7 +3308,7 @@
         <v>163</v>
       </c>
       <c r="C2" s="8">
-        <v>1</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3324,7 +3318,9 @@
       <c r="B3" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="6">
+        <v>0.47</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
@@ -3346,7 +3342,7 @@
       </c>
       <c r="C5" s="32">
         <f>IF((C2-C3)&gt;=0,ROUND((C2-C3)*100,0),"")</f>
-        <v>100</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3422,7 +3418,7 @@
         <v>167</v>
       </c>
       <c r="C12" s="8">
-        <v>7.91</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -3433,7 +3429,7 @@
         <v>168</v>
       </c>
       <c r="C13" s="6">
-        <v>7.86</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -3454,7 +3450,7 @@
       </c>
       <c r="C15" s="32">
         <f>IF((C12-C13)&gt;=0,ROUND((C12-C13)*100,0),"")</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3466,7 +3462,7 @@
       </c>
       <c r="C16" s="39" t="str">
         <f>IF(C15=0,"Permanece",IF(C15="","Baja","Sube"))</f>
-        <v>Sube</v>
+        <v>Permanece</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -3528,7 +3524,7 @@
         <v>113</v>
       </c>
       <c r="C22" s="8">
-        <v>0</v>
+        <v>56.7</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -3539,7 +3535,7 @@
         <v>114</v>
       </c>
       <c r="C23" s="6">
-        <v>55.9</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3550,7 +3546,7 @@
         <v>115</v>
       </c>
       <c r="C24" s="10">
-        <v>0</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -3583,29 +3579,29 @@
         <v>118</v>
       </c>
       <c r="C27" s="10">
-        <v>0</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="28" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>441</v>
+        <v>386</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="29" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -3616,7 +3612,7 @@
         <v>121</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>439</v>
+        <v>429</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3627,7 +3623,7 @@
         <v>122</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -3638,7 +3634,7 @@
         <v>127</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>391</v>
+        <v>429</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3649,30 +3645,26 @@
         <v>128</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>381</v>
+        <v>434</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="27" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>427</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>391</v>
-      </c>
+        <v>419</v>
+      </c>
+      <c r="C34" s="11"/>
     </row>
     <row r="35" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="27" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>428</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>381</v>
-      </c>
+        <v>420</v>
+      </c>
+      <c r="C35" s="12"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="28" t="s">
@@ -3682,7 +3674,7 @@
         <v>129</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>378</v>
+        <v>435</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3693,7 +3685,7 @@
         <v>130</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>379</v>
+        <v>436</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -3703,9 +3695,7 @@
       <c r="B38" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="C38" s="11" t="s">
-        <v>392</v>
-      </c>
+      <c r="C38" s="11"/>
     </row>
     <row r="39" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="29" t="s">
@@ -3714,11 +3704,9 @@
       <c r="B39" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="C39" s="12" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="12"/>
+    </row>
+    <row r="40" spans="1:3" ht="248.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="28" t="s">
         <v>65</v>
       </c>
@@ -3726,7 +3714,7 @@
         <v>119</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>393</v>
+        <v>437</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3737,7 +3725,7 @@
         <v>120</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>394</v>
+        <v>438</v>
       </c>
     </row>
   </sheetData>
@@ -3767,8 +3755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5F464D-9489-4499-83A6-0FFC57B0DDBD}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -3798,7 +3786,7 @@
         <v>155</v>
       </c>
       <c r="C2" s="8">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3809,7 +3797,7 @@
         <v>156</v>
       </c>
       <c r="C3" s="6">
-        <v>4.9000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3832,7 +3820,7 @@
       </c>
       <c r="C5" s="32">
         <f>IF((C2-C3)&gt;=0,ROUND((C2-C3)*100,0),"")</f>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3844,7 +3832,7 @@
       </c>
       <c r="C6" s="39" t="str">
         <f>IF(C5=0,"Permanece",IF(C5="","Baja","Sube"))</f>
-        <v>Sube</v>
+        <v>Permanece</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3852,10 +3840,10 @@
         <v>52</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="C7" s="8">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3863,10 +3851,10 @@
         <v>53</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="C8" s="6">
-        <v>48</v>
+        <v>8.6999999999999993</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3874,10 +3862,10 @@
         <v>54</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="C9" s="10">
-        <v>100</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -3885,10 +3873,10 @@
         <v>55</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="C10" s="6">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -3896,10 +3884,10 @@
         <v>57</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="C11" s="6">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3907,10 +3895,10 @@
         <v>56</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="C12" s="10">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -3921,7 +3909,7 @@
         <v>161</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3932,18 +3920,18 @@
         <v>162</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="182.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="28" t="s">
         <v>65</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>393</v>
+        <v>440</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3951,10 +3939,10 @@
         <v>66</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>394</v>
+        <v>432</v>
       </c>
     </row>
   </sheetData>
@@ -4316,7 +4304,7 @@
         <v>176</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -4327,7 +4315,7 @@
         <v>177</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4338,7 +4326,7 @@
         <v>178</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -4421,7 +4409,7 @@
         <v>200</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4618,7 +4606,7 @@
         <v>239</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -4640,7 +4628,7 @@
         <v>244</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4651,7 +4639,7 @@
         <v>243</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -4680,7 +4668,7 @@
         <v>245</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4702,7 +4690,7 @@
         <v>253</v>
       </c>
       <c r="C21" s="72" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4713,7 +4701,7 @@
         <v>254</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
   </sheetData>
@@ -4769,10 +4757,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="C2" s="74">
         <v>8.39</v>
@@ -4780,10 +4768,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="C3" s="73">
         <v>8.36</v>
@@ -4791,10 +4779,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>255</v>
@@ -4805,7 +4793,7 @@
         <v>44</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="C5" s="32">
         <f>IF((C2-C3)&gt;=0,ROUND((C2-C3)*100,0),"")</f>
@@ -4817,7 +4805,7 @@
         <v>45</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="C6" s="39" t="str">
         <f>IF(C5=0,"Permanece",IF(C5="","Baja","Sube"))</f>
@@ -4829,7 +4817,7 @@
         <v>52</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="C7" s="8">
         <v>0</v>
@@ -4840,7 +4828,7 @@
         <v>53</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="C8" s="6">
         <v>63.8</v>
@@ -4851,7 +4839,7 @@
         <v>54</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="C9" s="6">
         <v>0</v>
@@ -4862,7 +4850,7 @@
         <v>55</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="C10" s="6">
         <v>0</v>
@@ -4873,7 +4861,7 @@
         <v>57</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="C11" s="6">
         <v>0</v>
@@ -4884,7 +4872,7 @@
         <v>56</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="C12" s="10">
         <v>0</v>
@@ -4892,10 +4880,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="C13" s="11">
         <v>7.24</v>
@@ -4903,13 +4891,13 @@
     </row>
     <row r="14" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="198.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4917,10 +4905,10 @@
         <v>65</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4928,7 +4916,7 @@
         <v>66</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>377</v>
@@ -5317,13 +5305,13 @@
       </c>
       <c r="F25" s="54" t="str">
         <f>_xlfn.CONCAT(IF(OR(MAX(SANTALUCIA!C22:C24)&gt;$D$3,SUM(SANTALUCIA!C22:C24)&gt;$E$3),$F$3,IF(OR(MAX(SANTALUCIA!C22:C24)&gt;$D$4,SUM(SANTALUCIA!C22:C24)&gt;$E$4),$F$4,$F$5)),D25,$I$3,SUM(SANTALUCIA!C22:C24),$J$3,MAX(SANTALUCIA!C22:C24),$K$3)</f>
-        <v>En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Santa Lucía, donde en las últimas 72 horas se acumularon 55.9 mm y con un máximo de 55.9 mm/día.</v>
+        <v>En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Santa Lucía, donde en las últimas 72 horas se acumularon 69 mm y con un máximo de 56.7 mm/día.</v>
       </c>
       <c r="G25" s="54"/>
       <c r="H25" s="54"/>
       <c r="I25" s="66" t="str">
         <f>_xlfn.CONCAT($F$8,D25,IF(SANTALUCIA!C16=$E$8,$I$8,IF(SANTALUCIA!C16=$E$9,$I$9,$I$10)),$J$8,E25,". ")</f>
-        <v xml:space="preserve">Actualmente, el nivel del río Santa Lucía está en ascenso en la ciudad de Santa Lucía. </v>
+        <v xml:space="preserve">Actualmente, el nivel del río Santa Lucía se mantiene constante en la ciudad de Santa Lucía. </v>
       </c>
       <c r="J25" s="55" t="str">
         <f>_xlfn.CONCAT(F13,IF(SANTALUCIA!C36&gt;SANTALUCIA!C12,I13, IF(SANTALUCIA!C36=SANTALUCIA!C12,I14, I15)))</f>
@@ -5335,7 +5323,7 @@
       </c>
       <c r="L25" s="54" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Santa Lucía, donde en las últimas 72 horas se acumularon 55.9 mm y con un máximo de 55.9 mm/día. Actualmente, el nivel del río Santa Lucía está en ascenso en la ciudad de Santa Lucía.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  Existe una alta probabilidad de que el nivel supere al máximo registrado los días anteriores ( metros). </v>
+        <v xml:space="preserve">En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Santa Lucía, donde en las últimas 72 horas se acumularon 69 mm y con un máximo de 56.7 mm/día. Actualmente, el nivel del río Santa Lucía se mantiene constante en la ciudad de Santa Lucía.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  Existe una alta probabilidad de que el nivel supere al máximo registrado los días anteriores ( metros). </v>
       </c>
     </row>
     <row r="26" spans="3:13" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update status april 2025
</commit_message>
<xml_diff>
--- a/automatic docx/database_report.xlsx
+++ b/automatic docx/database_report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Sala_Situacion_Dinagua\automatic docx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9128F851-17F4-4471-AF17-4E0511066936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB75B6E-7C29-443D-AEDD-7D6BED9C6473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{83108E16-E9D6-4CCB-B5BE-A67101359CD3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{83108E16-E9D6-4CCB-B5BE-A67101359CD3}"/>
   </bookViews>
   <sheets>
     <sheet name="INICIO" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="434">
   <si>
     <t>fecha_emision</t>
   </si>
@@ -1161,63 +1161,6 @@
     <t xml:space="preserve">Estar atentos a los pronósticos meteorológicos que realiza el INUMET y a los próximos eventos de lluvia que se registren en la cuenca.   </t>
   </si>
   <si>
-    <t>Entre 9.0 a 9.5 m</t>
-  </si>
-  <si>
-    <t>30 mayo</t>
-  </si>
-  <si>
-    <t>02 - 03 mayo</t>
-  </si>
-  <si>
-    <t>Entre 9.8 - 9.3 m</t>
-  </si>
-  <si>
-    <t>Entre 8.2 a 8.6 m</t>
-  </si>
-  <si>
-    <t>Estar preparados ante la posibilidad de inundaciones que afecten a zona de vivienda.</t>
-  </si>
-  <si>
-    <t>10 mm en la parte alta de la cuenca</t>
-  </si>
-  <si>
-    <t>4 mm en la parte alta de la cuenca</t>
-  </si>
-  <si>
-    <t>35.8 mm en Alto río Negro</t>
-  </si>
-  <si>
-    <t>Menor a 3600</t>
-  </si>
-  <si>
-    <t>Menor a 4578</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estar atentos a los incrementos de nivel del río Negro en el tramo Represa Constitución y Mercedes. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actualmente se encuentra en tránsito una crecida del río Yí en el tramo Polanco del Yí y Durazno. En Sarandí Yí se registró el dia de ayer un nivel máximo de 5.44 m y actualmente se encuentra en descenso. En Polanco del Yí se encuentra en ascenso el nivel del río en una cota de 8.39 m (3 cm/h). En Durazno puente viejo se tiene un nivel de 9.14 m (Puente Ruta 5) y 8.05 m (en Puente Viejo). Estos niveles estan en ascenso y aun por debajo de la cota de seguridad (8.2 m en Durazno Puente Viejo). En base a estas condiciones se espera que se mantenga en ascenso el nivel del río Yí y superando la cota de seguridad en el transcurso del día. Actualmente el nivel máximo pronosticado para Durazno seria entre 8.2 a 8.6 metros en Durazno puente viejo para 02 o 03 de mayo. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">En las últimas horas no se registraron precipitaciones en la cuenca del río Cuareim. Actualmente, el nivel del río Cuareim se mantiene constante en la ciudad de Artigas.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, se prevé que el nivel siga en descenso en los próximos días.  </t>
-  </si>
-  <si>
-    <t>Menor a 4.0 m</t>
-  </si>
-  <si>
-    <t>entre 12,800 y 13,800</t>
-  </si>
-  <si>
-    <t>En las últimas horas se registraron bajos acumulados de precipitación en la cuenca del río Uruguay. Actualmente el nivel del río se mantiene con un descenso de nivel en el tramo Salto - Fray Bentos. Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, se prevé que se mantega la tendencia descendiente.</t>
-  </si>
-  <si>
-    <t>5.91 m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En las últimas horas no se registraron precipitaciones significativas en la cuenca del río Negro. UTE reporta que el nivel del río Negro en San Gregorio de Polanco podria descender los próximos dias, mientras que en Mercedes se espera para el 30-05-2024 un incremento de nivel que llegaria a un nivel de 5.91 m. </t>
-  </si>
-  <si>
     <t>último dato en Treinta y Tres</t>
   </si>
   <si>
@@ -1233,9 +1176,6 @@
     <t>fecha ocurrencia nivel máximo en Treinta y Tres</t>
   </si>
   <si>
-    <t xml:space="preserve">En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Yí, donde en las últimas 72 horas se acumularon 63.8 mm y con un máximo de 63.8 mm/día. Actualmente, el nivel del río Yí está en ascenso en la ciudad de Durazno.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  Existe una alta probabilidad de que el nivel supere al máximo registrado los días anteriores ( metros). </t>
-  </si>
-  <si>
     <t>nivel_actual_treintatres</t>
   </si>
   <si>
@@ -1281,9 +1221,6 @@
     <t>recomendacion_olimar</t>
   </si>
   <si>
-    <t>30 Octubre</t>
-  </si>
-  <si>
     <t>Pronostico hidrologico en San Ramón</t>
   </si>
   <si>
@@ -1335,37 +1272,79 @@
     <t>Menor a 2.0 m</t>
   </si>
   <si>
-    <t>Alrededor de 7 metros</t>
-  </si>
-  <si>
-    <t>Entre 04 y 05 de marzo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estar preparados a posibilidad de inundaciones y afectación a vivienda en San José. </t>
-  </si>
-  <si>
-    <t>Entre el 05 y 06 marzo</t>
-  </si>
-  <si>
     <t>05 de marzo</t>
   </si>
   <si>
-    <t>Menor a 4.5 m</t>
-  </si>
-  <si>
-    <t>Entre el 07 y 08 marzo</t>
-  </si>
-  <si>
-    <t>En la ultima semana se registraron 137 mm y 104.5 mm acumulado de lluvia en las subcuencas de los ríos Santa Lucia Chico y Grande, respectivamente. Se espera incrementos de nivel del río Santa Lucia Chico y el Santa Lucia desde el tramo de Paso Pache hasta Aguas Corrientes en los próximos días, dado que el mayor aporte vendría de ese lado de la cuenca (Santa Lucia Chico) que del río Santa Lucia Grande. Según datos que nos pasa la OSE, antes del evento Paso Severino estaba a un 84,4% de capacidad de almacenaje y buena parte de la crecida ayudaría a volver a llenar el embalse (actualmente está aumentando a 93,4% de volumen almacenado)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estar atentos al incremento del nivel del río Santa Lucia Grande y Chico. </t>
-  </si>
-  <si>
-    <t>Se registran incrementos significativos de nivel en los ríos San José, Santa Lucia Chico y los que drenan hasta el Río de la Plata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En la ultima semana se han registrado 127.5 mm de lluvia en la cuenca del río San Jose, registrandose entre las 7 hrs del 03-Marzo hasta las 7 hrs 04-Marzo un acumulado de 64 mm en promedio. Actualmente CECOED San José reporta un incremento del nivel del río San José cercano a los 7.3 metros, lo cual estaria superando la cota de seguridad (7.4 m) definido para la ciudad. Se debe estar atentos y estar preparados dado que el nivel máximo aun no ha llegado. </t>
+    <t>Menor a 3 metros</t>
+  </si>
+  <si>
+    <t>En las últimas horas se registraron bajos acumulados de precipitación en la cuenca del río Yí, donde en las últimas 72 horas se acumularon 4.3 mm y con un máximo de 4.3 mm/día. Actualmente, el nivel del río Yí se mantiene constante en la ciudad de Durazno.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, no se prevé incrementos de nivel que puedan generar inundaciones en la ciudad de Durazno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estar atentos a los pronósticos meteorológicos que realiza el INUMET    </t>
+  </si>
+  <si>
+    <t>Entre 9 y 10 mayo</t>
+  </si>
+  <si>
+    <t>Entre 10 y 11 mayo</t>
+  </si>
+  <si>
+    <t>Menor a 3.0 m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En las últimas 72 horas se acumularon 18.9 mm en la cuenca del río Santa Lucia. Actualmente, el nivel del río Santa Lucía se mantiene constante en la ciudad de Santa Lucía.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, no se prevé incrementos de nivel que puedan generar inundaciones. </t>
+  </si>
+  <si>
+    <t>Menor a 4 metros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En las últimas horas se registraron bajos acumulados de precipitación en la cuenca del río San José, donde en las últimas 72 horas se acumularon 18.9 mm. Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, no se esperan inundaciones en la ciudad de San José </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -</t>
+  </si>
+  <si>
+    <t>4 mm en cuenca incremental a Salto Grande</t>
+  </si>
+  <si>
+    <t>1 mm en cuenca incremental a Salto Grande</t>
+  </si>
+  <si>
+    <t>Entre 1,800 a 2,800 m3/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se observa que el nivel del río Uruguay en Paysandú permanence por debajo entre 0.50 a 0.54 metros. Debido a las precipitaciones pronosticadas, se espera incrementos de nivel en los afluentes al río Uruguay, tales como río Arapey y Daymán. </t>
+  </si>
+  <si>
+    <t>Entre 231 a 450 m3/s</t>
+  </si>
+  <si>
+    <t>Entre 2.54 a 624 m3/s</t>
+  </si>
+  <si>
+    <t>Menor a 3.5 m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En las últimas horas se registraron bajos acumulados de precipitación en la cuenca del Río Negro. No se prevé incrementos de nivel que puedan generar afectaciones en la parte baja del río Negro. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">En las últimas 72 horas se acumularon 4.3 mm y en la cuenca del río Olimar Grande. Actualmente, el nivel del río se mantiene constante en la ciudad de Treinta y Tres.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, no se prevé incrementos de nivel que puedan generar inundaciones en la ciudad de Treinta y Tres. </t>
+  </si>
+  <si>
+    <t>Rio Cuareim en ascenso pero con muy baja probabilidades de generar inundaciones en Artigas</t>
+  </si>
+  <si>
+    <t>Menor a 4.60 m</t>
+  </si>
+  <si>
+    <t>Menor a 8.20 m</t>
+  </si>
+  <si>
+    <t>Durante los últimos 3 días registró en promedio 62,5 mm en la cuenca del río Cuareim, con valores puntuales máximo de 85 mm en la parte alta de la cuenca. Las precipitaciones más fuertes se registraron en la cuenca vecina al río Cuareim (Ibicuí) que transita en río Grande do Sul (Brasil). Actualmente, se encuentra en ascenso el río Cuareim en las estaciones Artigas y Cuareim río, sin embargo se reduce la probabilidad de inundaciones en zona de vivienda en Artigas y la probabilidad de superar la cota de aviso (8 metros) es baja al momento de emitir este informe. Se espera que la onda de crecida llegue entre mañana y el domingo, pero no se espera mayores inconvenientes en la actividad cotidiana. Se actualizará el día de mañana.</t>
+  </si>
+  <si>
+    <t>Mantener el monitoreo en la red de estaciones de nivel del río Cuareim.</t>
   </si>
 </sst>
 </file>
@@ -2231,7 +2210,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="41">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2243,7 +2222,7 @@
       </c>
       <c r="C3" s="42">
         <f ca="1">TODAY()</f>
-        <v>45720</v>
+        <v>45786</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -2255,7 +2234,7 @@
       </c>
       <c r="C4" s="43">
         <f ca="1">$C$3-1</f>
-        <v>45719</v>
+        <v>45785</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2267,7 +2246,7 @@
       </c>
       <c r="C5" s="42">
         <f ca="1">$C$3-2</f>
-        <v>45718</v>
+        <v>45784</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -2279,7 +2258,7 @@
       </c>
       <c r="C6" s="43">
         <f ca="1">$C$3+1</f>
-        <v>45721</v>
+        <v>45787</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -2291,7 +2270,7 @@
       </c>
       <c r="C7" s="44">
         <f ca="1">$C$3+2</f>
-        <v>45722</v>
+        <v>45788</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2303,7 +2282,7 @@
       </c>
       <c r="C8" s="42">
         <f ca="1">$C$3+3</f>
-        <v>45723</v>
+        <v>45789</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2314,7 +2293,7 @@
         <v>172</v>
       </c>
       <c r="C9" s="45" t="s">
-        <v>439</v>
+        <v>429</v>
       </c>
     </row>
   </sheetData>
@@ -2439,8 +2418,8 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2470,7 +2449,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="74">
-        <v>4.67</v>
+        <v>1.1200000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2481,7 +2460,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="73">
-        <v>4.72</v>
+        <v>1.1200000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2491,9 +2470,9 @@
       <c r="B4" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="32" t="str">
+      <c r="C4" s="32">
         <f>IF((C2-C3)&gt;=0,ROUND((C2-C3)*100,0),"")</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2505,7 +2484,7 @@
       </c>
       <c r="C5" s="39" t="str">
         <f>IF(C4=0,"Permanece",IF(C4="","Baja","Sube"))</f>
-        <v>Baja</v>
+        <v>Permanece</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2516,7 +2495,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="74">
-        <v>8.39</v>
+        <v>1.54</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2527,7 +2506,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="73">
-        <v>8.36</v>
+        <v>1.54</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2550,7 +2529,7 @@
       </c>
       <c r="C9" s="32">
         <f>IF((C6-C7)&gt;=0,ROUND((C6-C7)*100,0),"")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2562,7 +2541,7 @@
       </c>
       <c r="C10" s="39" t="str">
         <f>IF(C9=0,"Permanece",IF(C9="","Baja","Sube"))</f>
-        <v>Sube</v>
+        <v>Permanece</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2573,7 +2552,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="74">
-        <v>8.0500000000000007</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2584,7 +2563,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="73">
-        <v>8.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2605,7 +2584,7 @@
       </c>
       <c r="C14" s="32">
         <f>IF((C11-C12)&gt;=0,ROUND((C11-C12)*100,0),"")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2617,7 +2596,7 @@
       </c>
       <c r="C15" s="39" t="str">
         <f>IF(C14=0,"Permanece",IF(C14="","Baja","Sube"))</f>
-        <v>Sube</v>
+        <v>Permanece</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2628,7 +2607,7 @@
         <v>13</v>
       </c>
       <c r="C16" s="73">
-        <v>9.14</v>
+        <v>1.91</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2639,7 +2618,7 @@
         <v>14</v>
       </c>
       <c r="C17" s="73">
-        <v>9.1</v>
+        <v>1.91</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2660,7 +2639,7 @@
       </c>
       <c r="C19" s="32">
         <f>IF((C16-C17)&gt;=0,ROUND((C16-C17)*100,0),"")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2672,7 +2651,7 @@
       </c>
       <c r="C20" s="39" t="str">
         <f>IF(C19=0,"Permanece",IF(C19="","Baja","Sube"))</f>
-        <v>Sube</v>
+        <v>Permanece</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2694,7 +2673,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="6">
-        <v>63.8</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2716,7 +2695,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="6">
-        <v>0</v>
+        <v>11.8</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2727,7 +2706,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="6">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2766,9 +2745,7 @@
       <c r="B29" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="11" t="s">
-        <v>372</v>
-      </c>
+      <c r="C29" s="11"/>
     </row>
     <row r="30" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="29" t="s">
@@ -2777,9 +2754,7 @@
       <c r="B30" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C30" s="12" t="s">
-        <v>373</v>
-      </c>
+      <c r="C30" s="12"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="28" t="s">
@@ -2789,7 +2764,7 @@
         <v>28</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>376</v>
+        <v>410</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2799,9 +2774,7 @@
       <c r="B32" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="12" t="s">
-        <v>374</v>
-      </c>
+      <c r="C32" s="12"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="28" t="s">
@@ -2811,7 +2784,7 @@
         <v>29</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>375</v>
+        <v>410</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2821,11 +2794,9 @@
       <c r="B34" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C34" s="12" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="281.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="12"/>
+    </row>
+    <row r="35" spans="1:3" ht="182.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="28" t="s">
         <v>65</v>
       </c>
@@ -2833,7 +2804,7 @@
         <v>39</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>384</v>
+        <v>411</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2844,7 +2815,7 @@
         <v>41</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>377</v>
+        <v>412</v>
       </c>
     </row>
   </sheetData>
@@ -2875,7 +2846,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D9A6E30-A876-45F0-8067-30FAF0E80436}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A12" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -2906,7 +2877,7 @@
         <v>83</v>
       </c>
       <c r="C2" s="6">
-        <v>4.2300000000000004</v>
+        <v>4.7699999999999996</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2917,7 +2888,7 @@
         <v>84</v>
       </c>
       <c r="C3" s="6">
-        <v>4.2300000000000004</v>
+        <v>4.79</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2938,9 +2909,9 @@
       <c r="B5" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="32" t="str">
         <f>IF((C2-C3)&gt;=0,ROUND((C2-C3)*100,0),"")</f>
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2952,7 +2923,7 @@
       </c>
       <c r="C6" s="39" t="str">
         <f>IF(C5=0,"Permanece",IF(C5="","Baja","Sube"))</f>
-        <v>Permanece</v>
+        <v>Baja</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2963,7 +2934,7 @@
         <v>89</v>
       </c>
       <c r="C7" s="6">
-        <v>1.53</v>
+        <v>1.95</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2974,7 +2945,7 @@
         <v>90</v>
       </c>
       <c r="C8" s="6">
-        <v>1.53</v>
+        <v>1.83</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2997,7 +2968,7 @@
       </c>
       <c r="C10" s="32">
         <f>IF((C7-C8)&gt;=0,ROUND((C7-C8)*100,0),"")</f>
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3009,7 +2980,7 @@
       </c>
       <c r="C11" s="39" t="str">
         <f>IF(C10=0,"Permanece",IF(C10="","Baja","Sube"))</f>
-        <v>Permanece</v>
+        <v>Sube</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -3020,7 +2991,7 @@
         <v>95</v>
       </c>
       <c r="C12" s="6">
-        <v>2.56</v>
+        <v>4.5199999999999996</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -3031,7 +3002,7 @@
         <v>96</v>
       </c>
       <c r="C13" s="6">
-        <v>2.56</v>
+        <v>4.37</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -3054,7 +3025,7 @@
       </c>
       <c r="C15" s="32">
         <f>IF((C12-C13)&gt;=0,ROUND((C12-C13)*100,0),"")</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3066,7 +3037,7 @@
       </c>
       <c r="C16" s="39" t="str">
         <f>IF(C15=0,"Permanece",IF(C15="","Baja","Sube"))</f>
-        <v>Permanece</v>
+        <v>Sube</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -3077,7 +3048,7 @@
         <v>75</v>
       </c>
       <c r="C17" s="8">
-        <v>0</v>
+        <v>24.2</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -3088,7 +3059,7 @@
         <v>76</v>
       </c>
       <c r="C18" s="6">
-        <v>0</v>
+        <v>37.700000000000003</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -3099,7 +3070,7 @@
         <v>77</v>
       </c>
       <c r="C19" s="6">
-        <v>0</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -3110,7 +3081,7 @@
         <v>78</v>
       </c>
       <c r="C20" s="6">
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -3142,7 +3113,9 @@
       <c r="B23" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C23" s="75"/>
+      <c r="C23" s="75" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="24" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="29" t="s">
@@ -3151,7 +3124,9 @@
       <c r="B24" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C24" s="11"/>
+      <c r="C24" s="11" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="25" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="28" t="s">
@@ -3160,7 +3135,9 @@
       <c r="B25" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C25" s="11"/>
+      <c r="C25" s="11" t="s">
+        <v>430</v>
+      </c>
     </row>
     <row r="26" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="29" t="s">
@@ -3169,7 +3146,9 @@
       <c r="B26" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C26" s="11"/>
+      <c r="C26" s="11" t="s">
+        <v>413</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
@@ -3178,7 +3157,9 @@
       <c r="B27" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C27" s="11"/>
+      <c r="C27" s="11" t="s">
+        <v>431</v>
+      </c>
     </row>
     <row r="28" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="29" t="s">
@@ -3187,9 +3168,11 @@
       <c r="B28" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C28" s="12"/>
-    </row>
-    <row r="29" spans="1:11" ht="132.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="12" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="281.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="28" t="s">
         <v>65</v>
       </c>
@@ -3197,7 +3180,7 @@
         <v>81</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>385</v>
+        <v>432</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3208,7 +3191,7 @@
         <v>82</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>257</v>
+        <v>433</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -3278,7 +3261,7 @@
   <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -3308,7 +3291,7 @@
         <v>163</v>
       </c>
       <c r="C2" s="8">
-        <v>0.49</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3319,7 +3302,7 @@
         <v>164</v>
       </c>
       <c r="C3" s="6">
-        <v>0.47</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3342,7 +3325,7 @@
       </c>
       <c r="C5" s="32">
         <f>IF((C2-C3)&gt;=0,ROUND((C2-C3)*100,0),"")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3354,7 +3337,7 @@
       </c>
       <c r="C6" s="39" t="str">
         <f>IF(C5=0,"Permanece",IF(C5="","Baja","Sube"))</f>
-        <v>Sube</v>
+        <v>Permanece</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3364,7 +3347,9 @@
       <c r="B7" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="C7" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
@@ -3373,7 +3358,9 @@
       <c r="B8" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
@@ -3524,7 +3511,7 @@
         <v>113</v>
       </c>
       <c r="C22" s="8">
-        <v>56.7</v>
+        <v>11.1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -3535,7 +3522,7 @@
         <v>114</v>
       </c>
       <c r="C23" s="6">
-        <v>7.9</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3546,7 +3533,7 @@
         <v>115</v>
       </c>
       <c r="C24" s="10">
-        <v>4.4000000000000004</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -3557,7 +3544,7 @@
         <v>116</v>
       </c>
       <c r="C25" s="6">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -3579,30 +3566,28 @@
         <v>118</v>
       </c>
       <c r="C27" s="10">
-        <v>1.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="28" t="s">
-        <v>413</v>
+        <v>392</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>415</v>
+        <v>394</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>386</v>
+        <v>408</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="29" t="s">
-        <v>414</v>
+        <v>393</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>416</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>433</v>
-      </c>
+        <v>395</v>
+      </c>
+      <c r="C29" s="12"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="28" t="s">
@@ -3612,7 +3597,7 @@
         <v>121</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>429</v>
+        <v>408</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3622,9 +3607,7 @@
       <c r="B31" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="C31" s="12" t="s">
-        <v>434</v>
-      </c>
+      <c r="C31" s="12"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
@@ -3634,7 +3617,7 @@
         <v>127</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>429</v>
+        <v>408</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3645,24 +3628,24 @@
         <v>128</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>434</v>
+        <v>409</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="27" t="s">
-        <v>417</v>
+        <v>396</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>419</v>
+        <v>398</v>
       </c>
       <c r="C34" s="11"/>
     </row>
     <row r="35" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="27" t="s">
-        <v>418</v>
+        <v>397</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>420</v>
+        <v>399</v>
       </c>
       <c r="C35" s="12"/>
     </row>
@@ -3674,7 +3657,7 @@
         <v>129</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>435</v>
+        <v>415</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3684,9 +3667,7 @@
       <c r="B37" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="C37" s="12" t="s">
-        <v>436</v>
-      </c>
+      <c r="C37" s="12"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="28" t="s">
@@ -3706,7 +3687,7 @@
       </c>
       <c r="C39" s="12"/>
     </row>
-    <row r="40" spans="1:3" ht="248.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="132.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="28" t="s">
         <v>65</v>
       </c>
@@ -3714,10 +3695,10 @@
         <v>119</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="30" t="s">
         <v>66</v>
       </c>
@@ -3725,7 +3706,7 @@
         <v>120</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>438</v>
+        <v>371</v>
       </c>
     </row>
   </sheetData>
@@ -3755,8 +3736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5F464D-9489-4499-83A6-0FFC57B0DDBD}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -3840,10 +3821,10 @@
         <v>52</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>421</v>
+        <v>400</v>
       </c>
       <c r="C7" s="8">
-        <v>64</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3851,10 +3832,10 @@
         <v>53</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>422</v>
+        <v>401</v>
       </c>
       <c r="C8" s="6">
-        <v>8.6999999999999993</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3862,10 +3843,10 @@
         <v>54</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>423</v>
+        <v>402</v>
       </c>
       <c r="C9" s="10">
-        <v>5.9</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -3873,10 +3854,10 @@
         <v>55</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>424</v>
+        <v>403</v>
       </c>
       <c r="C10" s="6">
-        <v>0</v>
+        <v>23.8</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -3884,10 +3865,10 @@
         <v>57</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>425</v>
+        <v>404</v>
       </c>
       <c r="C11" s="6">
-        <v>0</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3895,7 +3876,7 @@
         <v>56</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>426</v>
+        <v>405</v>
       </c>
       <c r="C12" s="10">
         <v>0</v>
@@ -3909,7 +3890,7 @@
         <v>161</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>430</v>
+        <v>417</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3919,30 +3900,28 @@
       <c r="B14" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="182.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="12"/>
+    </row>
+    <row r="15" spans="1:3" ht="116.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="28" t="s">
         <v>65</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>427</v>
+        <v>406</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
         <v>66</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>428</v>
+        <v>407</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>432</v>
+        <v>371</v>
       </c>
     </row>
   </sheetData>
@@ -3972,7 +3951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2155F922-1445-4239-A643-A9F5E09853DC}">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
@@ -4004,7 +3983,7 @@
         <v>209</v>
       </c>
       <c r="C2" s="74">
-        <v>7.8</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4015,7 +3994,7 @@
         <v>210</v>
       </c>
       <c r="C3" s="73">
-        <v>7.78</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -4038,7 +4017,7 @@
       </c>
       <c r="C5" s="32">
         <f>IF((C2-C3)&gt;=0,ROUND((C2-C3)*100,0),"")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D5" s="57"/>
     </row>
@@ -4051,7 +4030,7 @@
       </c>
       <c r="C6" s="39" t="str">
         <f>IF(C5=0,"Permanece",IF(C5="","Baja","Sube"))</f>
-        <v>Sube</v>
+        <v>Permanece</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -4062,7 +4041,7 @@
         <v>213</v>
       </c>
       <c r="C7" s="74">
-        <v>5.65</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -4073,7 +4052,7 @@
         <v>214</v>
       </c>
       <c r="C8" s="73">
-        <v>5.65</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -4120,7 +4099,7 @@
         <v>180</v>
       </c>
       <c r="C12" s="74">
-        <v>9.73</v>
+        <v>3.13</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -4131,7 +4110,7 @@
         <v>181</v>
       </c>
       <c r="C13" s="73">
-        <v>9.73</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -4154,7 +4133,7 @@
       </c>
       <c r="C15" s="32">
         <f>IF((C12-C13)&gt;=0,ROUND((C12-C13)*100,0),"")</f>
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4166,7 +4145,7 @@
       </c>
       <c r="C16" s="39" t="str">
         <f>IF(C15=0,"Permanece",IF(C15="","Baja","Sube"))</f>
-        <v>Permanece</v>
+        <v>Sube</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -4177,7 +4156,7 @@
         <v>217</v>
       </c>
       <c r="C17" s="74">
-        <v>5.25</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -4188,7 +4167,7 @@
         <v>218</v>
       </c>
       <c r="C18" s="73">
-        <v>5.25</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -4198,8 +4177,8 @@
       <c r="B19" s="5" t="s">
         <v>325</v>
       </c>
-      <c r="C19" s="6">
-        <v>7.89</v>
+      <c r="C19" s="6" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -4209,9 +4188,9 @@
       <c r="B20" s="31" t="s">
         <v>219</v>
       </c>
-      <c r="C20" s="32">
+      <c r="C20" s="32" t="str">
         <f>IF((C17-C18)&gt;=0,ROUND((C17-C18)*100,0),"")</f>
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4223,7 +4202,7 @@
       </c>
       <c r="C21" s="39" t="str">
         <f>IF(C20=0,"Permanece",IF(C20="","Baja","Sube"))</f>
-        <v>Permanece</v>
+        <v>Baja</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -4234,7 +4213,7 @@
         <v>221</v>
       </c>
       <c r="C22" s="74">
-        <v>2.78</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -4245,7 +4224,7 @@
         <v>222</v>
       </c>
       <c r="C23" s="73">
-        <v>2.88</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -4292,8 +4271,8 @@
       <c r="B27" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="C27" s="8">
-        <v>0</v>
+      <c r="C27" s="8" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -4304,7 +4283,7 @@
         <v>176</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>378</v>
+        <v>420</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -4315,7 +4294,7 @@
         <v>177</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>379</v>
+        <v>421</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4326,7 +4305,7 @@
         <v>178</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>387</v>
+        <v>422</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -4401,7 +4380,7 @@
       </c>
       <c r="C38" s="12"/>
     </row>
-    <row r="39" spans="1:3" ht="132.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="99.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="28" t="s">
         <v>65</v>
       </c>
@@ -4409,10 +4388,10 @@
         <v>200</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="30" t="s">
         <v>66</v>
       </c>
@@ -4420,7 +4399,7 @@
         <v>225</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>257</v>
+        <v>371</v>
       </c>
     </row>
   </sheetData>
@@ -4451,7 +4430,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -4481,7 +4460,7 @@
         <v>228</v>
       </c>
       <c r="C2" s="8">
-        <v>11.65</v>
+        <v>5.71</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -4492,7 +4471,7 @@
         <v>229</v>
       </c>
       <c r="C3" s="6">
-        <v>11.64</v>
+        <v>5.72</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -4513,9 +4492,9 @@
       <c r="B5" s="31" t="s">
         <v>230</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="32" t="str">
         <f>IF((C2-C3)&gt;=0,ROUND((C2-C3)*100,0),"")</f>
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4527,7 +4506,7 @@
       </c>
       <c r="C6" s="39" t="str">
         <f>IF(C5=0,"Permanece",IF(C5="","Baja","Sube"))</f>
-        <v>Sube</v>
+        <v>Baja</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -4538,7 +4517,7 @@
         <v>234</v>
       </c>
       <c r="C7" s="8">
-        <v>5.87</v>
+        <v>1.1100000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4549,7 +4528,7 @@
         <v>235</v>
       </c>
       <c r="C8" s="6">
-        <v>5.87</v>
+        <v>1.1200000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -4570,9 +4549,9 @@
       <c r="B10" s="31" t="s">
         <v>236</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="32" t="str">
         <f>IF((C7-C8)&gt;=0,ROUND((C7-C8)*100,0),"")</f>
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4584,7 +4563,7 @@
       </c>
       <c r="C11" s="39" t="str">
         <f>IF(C10=0,"Permanece",IF(C10="","Baja","Sube"))</f>
-        <v>Permanece</v>
+        <v>Baja</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -4595,7 +4574,7 @@
         <v>238</v>
       </c>
       <c r="C12" s="8">
-        <v>0</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -4605,8 +4584,8 @@
       <c r="B13" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>380</v>
+      <c r="C13" s="6">
+        <v>5.6</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -4617,7 +4596,7 @@
         <v>240</v>
       </c>
       <c r="C14" s="6">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -4628,7 +4607,7 @@
         <v>244</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>381</v>
+        <v>424</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4639,7 +4618,7 @@
         <v>243</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>382</v>
+        <v>425</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -4668,7 +4647,7 @@
         <v>245</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>389</v>
+        <v>426</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4678,11 +4657,9 @@
       <c r="B20" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="132.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="12"/>
+    </row>
+    <row r="21" spans="1:3" ht="83.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="28" t="s">
         <v>65</v>
       </c>
@@ -4690,7 +4667,7 @@
         <v>253</v>
       </c>
       <c r="C21" s="72" t="s">
-        <v>390</v>
+        <v>427</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4701,7 +4678,7 @@
         <v>254</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>383</v>
+        <v>371</v>
       </c>
     </row>
   </sheetData>
@@ -4733,7 +4710,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -4757,32 +4734,32 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>391</v>
+        <v>372</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="C2" s="74">
-        <v>8.39</v>
+        <v>-0.22</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>392</v>
+        <v>373</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>398</v>
+        <v>378</v>
       </c>
       <c r="C3" s="73">
-        <v>8.36</v>
+        <v>-0.22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>393</v>
+        <v>374</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>399</v>
+        <v>379</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>255</v>
@@ -4793,11 +4770,11 @@
         <v>44</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>400</v>
+        <v>380</v>
       </c>
       <c r="C5" s="32">
         <f>IF((C2-C3)&gt;=0,ROUND((C2-C3)*100,0),"")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4805,11 +4782,11 @@
         <v>45</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>401</v>
+        <v>381</v>
       </c>
       <c r="C6" s="39" t="str">
         <f>IF(C5=0,"Permanece",IF(C5="","Baja","Sube"))</f>
-        <v>Sube</v>
+        <v>Permanece</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -4817,7 +4794,7 @@
         <v>52</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="C7" s="8">
         <v>0</v>
@@ -4828,10 +4805,10 @@
         <v>53</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="C8" s="6">
-        <v>63.8</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -4839,7 +4816,7 @@
         <v>54</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
       <c r="C9" s="6">
         <v>0</v>
@@ -4850,10 +4827,10 @@
         <v>55</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>405</v>
+        <v>385</v>
       </c>
       <c r="C10" s="6">
-        <v>0</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -4861,10 +4838,10 @@
         <v>57</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>406</v>
+        <v>386</v>
       </c>
       <c r="C11" s="6">
-        <v>0</v>
+        <v>17.2</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4872,54 +4849,52 @@
         <v>56</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>407</v>
+        <v>387</v>
       </c>
       <c r="C12" s="10">
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="s">
-        <v>394</v>
+        <v>375</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>409</v>
-      </c>
-      <c r="C13" s="11">
-        <v>7.24</v>
+        <v>389</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29" t="s">
-        <v>395</v>
+        <v>376</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>408</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="198.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>388</v>
+      </c>
+      <c r="C14" s="12"/>
+    </row>
+    <row r="15" spans="1:3" ht="149.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="28" t="s">
         <v>65</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>410</v>
+        <v>390</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
         <v>66</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>411</v>
+        <v>391</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
     </row>
   </sheetData>
@@ -5239,13 +5214,13 @@
       </c>
       <c r="F23" s="54" t="str">
         <f>_xlfn.CONCAT(IF(OR(MAX(YI!C21:C23)&gt;$D$3,SUM(YI!C21:C23)&gt;$E$3),$F$3,IF(OR(MAX(YI!C21:C23)&gt;$D$4,SUM(YI!C21:C23)&gt;$E$4),$F$4,$F$5)),D23,$I$3,SUM(YI!C21:C23),$J$3,MAX(YI!C21:C23),$K$3)</f>
-        <v>En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Yí, donde en las últimas 72 horas se acumularon 63.8 mm y con un máximo de 63.8 mm/día.</v>
+        <v>En las últimas horas se registraron bajos acumulados de precipitación en la cuenca del río Yí, donde en las últimas 72 horas se acumularon 4.3 mm y con un máximo de 4.3 mm/día.</v>
       </c>
       <c r="G23" s="54"/>
       <c r="H23" s="54"/>
       <c r="I23" s="54" t="str">
         <f>_xlfn.CONCAT($F$8,D23,IF(YI!C15=$E$8,$I$8,IF(YI!C15=$E$9,$I$9,$I$10)),$J$8,E23,". ")</f>
-        <v xml:space="preserve">Actualmente, el nivel del río Yí está en ascenso en la ciudad de Durazno. </v>
+        <v xml:space="preserve">Actualmente, el nivel del río Yí se mantiene constante en la ciudad de Durazno. </v>
       </c>
       <c r="J23" s="54" t="str">
         <f>_xlfn.CONCAT(F13,IF(YI!C31&gt;YI!C11,I13, IF(YI!C31=YI!C11,I14, I15)))</f>
@@ -5257,7 +5232,7 @@
       </c>
       <c r="L23" s="54" t="str">
         <f>+_xlfn.CONCAT(F23," ",I23, " ",J23," ",K23)</f>
-        <v xml:space="preserve">En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Yí, donde en las últimas 72 horas se acumularon 63.8 mm y con un máximo de 63.8 mm/día. Actualmente, el nivel del río Yí está en ascenso en la ciudad de Durazno.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  Existe una alta probabilidad de que el nivel supere al máximo registrado los días anteriores ( metros). </v>
+        <v xml:space="preserve">En las últimas horas se registraron bajos acumulados de precipitación en la cuenca del río Yí, donde en las últimas 72 horas se acumularon 4.3 mm y con un máximo de 4.3 mm/día. Actualmente, el nivel del río Yí se mantiene constante en la ciudad de Durazno.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  Existe una alta probabilidad de que el nivel supere al máximo registrado los días anteriores ( metros). </v>
       </c>
     </row>
     <row r="24" spans="3:13" ht="82.5" x14ac:dyDescent="0.3">
@@ -5272,17 +5247,17 @@
       </c>
       <c r="F24" s="55" t="str">
         <f>_xlfn.CONCAT(IF(OR(MAX(CUAREIM!C17:C19)&gt;$D$3,SUM(CUAREIM!C17:C19)&gt;$E$3),$F$3,IF(OR(MAX(CUAREIM!C17:C19)&gt;$D$4,SUM(CUAREIM!C17:C19)&gt;$E$4),$F$4,$F$5)),D24,$I$3,SUM(CUAREIM!C17:C19),$J$3,MAX(CUAREIM!C17:C19),$K$3)</f>
-        <v>En las últimas horas se registraron bajos acumulados de precipitación en la cuenca del río Cuareim, donde en las últimas 72 horas se acumularon 0 mm y con un máximo de 0 mm/día.</v>
+        <v>En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Cuareim, donde en las últimas 72 horas se acumularon 62.5 mm y con un máximo de 37.7 mm/día.</v>
       </c>
       <c r="G24" s="55"/>
       <c r="H24" s="55"/>
       <c r="I24" s="66" t="str">
         <f>_xlfn.CONCAT($F$8,D24,IF(CUAREIM!C16=$E$8,$I$8,IF(CUAREIM!C16=$E$9,$I$9,$I$10)),$J$8,E24,". ")</f>
-        <v xml:space="preserve">Actualmente, el nivel del río Cuareim se mantiene constante en la ciudad de Artigas. </v>
+        <v xml:space="preserve">Actualmente, el nivel del río Cuareim está en ascenso en la ciudad de Artigas. </v>
       </c>
       <c r="J24" s="55" t="str">
         <f>_xlfn.CONCAT(F13,IF(CUAREIM!C27&gt;CUAREIM!C12,I13, IF(CUAREIM!C27=CUAREIM!C12,I14, I15)))</f>
-        <v xml:space="preserve">Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, se prevé que el nivel descienda en los próximos días. </v>
+        <v xml:space="preserve">Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días. </v>
       </c>
       <c r="K24" s="54" t="str">
         <f>IF(CUAREIM!C14="-","",IF(CUAREIM!C27&gt;CUAREIM!C14,_xlfn.CONCAT(F18,CUAREIM!C14,I18),_xlfn.CONCAT(F19,CUAREIM!C14,I19)))</f>
@@ -5290,7 +5265,7 @@
       </c>
       <c r="L24" s="54" t="str">
         <f t="shared" ref="L24:L30" si="0">+_xlfn.CONCAT(F24," ",I24, " ",J24," ",K24)</f>
-        <v xml:space="preserve">En las últimas horas se registraron bajos acumulados de precipitación en la cuenca del río Cuareim, donde en las últimas 72 horas se acumularon 0 mm y con un máximo de 0 mm/día. Actualmente, el nivel del río Cuareim se mantiene constante en la ciudad de Artigas.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, se prevé que el nivel descienda en los próximos días.  </v>
+        <v xml:space="preserve">En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Cuareim, donde en las últimas 72 horas se acumularon 62.5 mm y con un máximo de 37.7 mm/día. Actualmente, el nivel del río Cuareim está en ascenso en la ciudad de Artigas.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  </v>
       </c>
     </row>
     <row r="25" spans="3:13" ht="99" x14ac:dyDescent="0.3">
@@ -5305,7 +5280,7 @@
       </c>
       <c r="F25" s="54" t="str">
         <f>_xlfn.CONCAT(IF(OR(MAX(SANTALUCIA!C22:C24)&gt;$D$3,SUM(SANTALUCIA!C22:C24)&gt;$E$3),$F$3,IF(OR(MAX(SANTALUCIA!C22:C24)&gt;$D$4,SUM(SANTALUCIA!C22:C24)&gt;$E$4),$F$4,$F$5)),D25,$I$3,SUM(SANTALUCIA!C22:C24),$J$3,MAX(SANTALUCIA!C22:C24),$K$3)</f>
-        <v>En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Santa Lucía, donde en las últimas 72 horas se acumularon 69 mm y con un máximo de 56.7 mm/día.</v>
+        <v>En las últimas horas se registraron bajos acumulados de precipitación en la cuenca del río Santa Lucía, donde en las últimas 72 horas se acumularon 18.9 mm y con un máximo de 11.1 mm/día.</v>
       </c>
       <c r="G25" s="54"/>
       <c r="H25" s="54"/>
@@ -5323,7 +5298,7 @@
       </c>
       <c r="L25" s="54" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">En las últimas horas se registraron acumulados de precipitación moderados en la cuenca del río Santa Lucía, donde en las últimas 72 horas se acumularon 69 mm y con un máximo de 56.7 mm/día. Actualmente, el nivel del río Santa Lucía se mantiene constante en la ciudad de Santa Lucía.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  Existe una alta probabilidad de que el nivel supere al máximo registrado los días anteriores ( metros). </v>
+        <v xml:space="preserve">En las últimas horas se registraron bajos acumulados de precipitación en la cuenca del río Santa Lucía, donde en las últimas 72 horas se acumularon 18.9 mm y con un máximo de 11.1 mm/día. Actualmente, el nivel del río Santa Lucía se mantiene constante en la ciudad de Santa Lucía.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  Existe una alta probabilidad de que el nivel supere al máximo registrado los días anteriores ( metros). </v>
       </c>
     </row>
     <row r="26" spans="3:13" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -5342,7 +5317,7 @@
       </c>
       <c r="I26" s="66" t="str">
         <f>IF(AND(URUGUAY!$C$11=$E$8,URUGUAY!$C$16=$E$8,URUGUAY!$C$21=$E$8,URUGUAY!$C$26=$E$8),_xlfn.CONCAT($F$8,$D$26,$I$8,$J$9," ",E26,", ",E27,", ",E28," y ",Tablas!E29,"."),IF(AND(URUGUAY!$C$11=$E$9,URUGUAY!$C$16=$E$9,URUGUAY!$C$21=$E$9,URUGUAY!$C$26=$E$9),_xlfn.CONCAT($F$8,$D$26,$I$9,$J$9," ",E26,", ",E27,", ",E28," y ",E29,"."),IF(AND(URUGUAY!$C$11=$E$10,URUGUAY!$C$16=$E$10,URUGUAY!$C$21=$E$10,URUGUAY!$C$26=$E$10),_xlfn.CONCAT($F$8,$D$26,$I$10,$J$9," ",E26,", ",E27,", ",E28," y ",E29,"."),_xlfn.CONCAT($F$8,D26,I27,I28,I29))))</f>
-        <v>Actualmente, el nivel del río Uruguay está en ascenso en la ciudad de ; se mantiene constante en las ciudades de Bella Unión Salto Paysandú; está en descenso en la ciudad de  Fray Bentos.</v>
+        <v>Actualmente, el nivel del río Uruguay está en ascenso en la ciudad de  Salto; se mantiene constante en la ciudad de  Bella Unión; está en descenso en las ciudades de Paysandú Fray Bentos.</v>
       </c>
       <c r="J26" s="77" t="str">
         <f>_xlfn.CONCAT(F13,IF(AND(URUGUAY!C31&gt;URUGUAY!C7, URUGUAY!C33&gt;URUGUAY!C12, URUGUAY!C35&gt;URUGUAY!C17, URUGUAY!C37&gt;URUGUAY!C22),I13, IF(AND(URUGUAY!C31=URUGUAY!C7, URUGUAY!C33=URUGUAY!C12, URUGUAY!C35=URUGUAY!C17, URUGUAY!C37=URUGUAY!C22),I14, I15)))</f>
@@ -5350,11 +5325,11 @@
       </c>
       <c r="K26" s="77" t="str">
         <f>IF(AND(URUGUAY!C9="-", URUGUAY!C14="-", URUGUAY!C19="-", URUGUAY!C24="-"),"",IF(OR(URUGUAY!C31&gt;URUGUAY!C9, URUGUAY!C33&gt;URUGUAY!C14, URUGUAY!C35&gt;URUGUAY!C19,URUGUAY!C37&gt;URUGUAY!C24),_xlfn.CONCAT(F18,IF(URUGUAY!C9&lt;&gt;"-",_xlfn.CONCAT(URUGUAY!C9,"m en ",E26," "),""), IF(URUGUAY!C14&lt;&gt;"-",_xlfn.CONCAT(URUGUAY!C14, "m en ",E27," "),""),IF(URUGUAY!C19&lt;&gt;"-",_xlfn.CONCAT(URUGUAY!C19,"m en ",E28," "),""),IF(URUGUAY!C24&lt;&gt;"-",_xlfn.CONCAT(URUGUAY!C24,"m en ",E29),""),")."),_xlfn.CONCAT(F19,IF(URUGUAY!C9&lt;&gt;"-",_xlfn.CONCAT(URUGUAY!C9,"m en ",E26," "),""), IF(URUGUAY!C14&lt;&gt;"-",_xlfn.CONCAT(URUGUAY!C14, "m en ",E27," "),""),IF(URUGUAY!C19&lt;&gt;"-",_xlfn.CONCAT(URUGUAY!C19,"m en ",E28," "),""),IF(URUGUAY!C24&lt;&gt;"-",_xlfn.CONCAT(URUGUAY!C24,"m en ",E29),""),", pero no se puede descartar en su totalidad.")))</f>
-        <v>Existe una baja probabilidad de que el nivel supere al máximo registrado los días anteriores (7.89m en Paysandú , pero no se puede descartar en su totalidad.</v>
+        <v>Existe una baja probabilidad de que el nivel supere al máximo registrado los días anteriores ( -m en Paysandú , pero no se puede descartar en su totalidad.</v>
       </c>
       <c r="L26" s="77" t="str">
         <f t="shared" si="0"/>
-        <v>En las últimas horas se registraron bajos acumulados de precipitación en la cuenca del río Uruguay, donde en las últimas 72 horas se acumularon 0 mm y con un máximo de 0 mm/día. Actualmente, el nivel del río Uruguay está en ascenso en la ciudad de ; se mantiene constante en las ciudades de Bella Unión Salto Paysandú; está en descenso en la ciudad de  Fray Bentos. Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, se prevé que el nivel descienda en los próximos días.  Existe una baja probabilidad de que el nivel supere al máximo registrado los días anteriores (7.89m en Paysandú , pero no se puede descartar en su totalidad.</v>
+        <v>En las últimas horas se registraron bajos acumulados de precipitación en la cuenca del río Uruguay, donde en las últimas 72 horas se acumularon 0 mm y con un máximo de 0 mm/día. Actualmente, el nivel del río Uruguay está en ascenso en la ciudad de  Salto; se mantiene constante en la ciudad de  Bella Unión; está en descenso en las ciudades de Paysandú Fray Bentos. Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, se prevé que el nivel descienda en los próximos días.  Existe una baja probabilidad de que el nivel supere al máximo registrado los días anteriores ( -m en Paysandú , pero no se puede descartar en su totalidad.</v>
       </c>
     </row>
     <row r="27" spans="3:13" x14ac:dyDescent="0.3">
@@ -5366,15 +5341,15 @@
       <c r="F27" s="76"/>
       <c r="G27" s="60">
         <f>SUM(URUGUAY!$C$11=Tablas!E8, URUGUAY!$C$16=Tablas!E8,URUGUAY!$C$21=Tablas!E8,URUGUAY!$C$26=Tablas!E8)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27" s="61" t="str">
         <f>_xlfn.CONCAT(IF(URUGUAY!$C$11=Tablas!E8,_xlfn.CONCAT(" ",$E$26,),""),IF(URUGUAY!$C$16=Tablas!E8,_xlfn.CONCAT(" ",$E$27),""),IF(URUGUAY!$C$21=Tablas!E8,_xlfn.CONCAT(" ",$E$28),""),IF(URUGUAY!$C$26=Tablas!E8,_xlfn.CONCAT(" ",$E$29),""))</f>
-        <v/>
+        <v xml:space="preserve"> Salto</v>
       </c>
       <c r="I27" s="67" t="str">
         <f>_xlfn.CONCAT(I8,IF(G27&gt;1,$J$9,$J$8),H27, IF(G27=4,".", ";"))</f>
-        <v xml:space="preserve"> está en ascenso en la ciudad de ;</v>
+        <v xml:space="preserve"> está en ascenso en la ciudad de  Salto;</v>
       </c>
       <c r="J27" s="77"/>
       <c r="K27" s="77"/>
@@ -5389,21 +5364,21 @@
       <c r="F28" s="76"/>
       <c r="G28" s="60">
         <f>SUM(URUGUAY!$C$11=Tablas!E9, URUGUAY!$C$16=Tablas!E9,URUGUAY!$C$21=Tablas!E9,URUGUAY!$C$26=Tablas!E9)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H28" s="61" t="str">
         <f>_xlfn.CONCAT(IF(URUGUAY!$C$11=Tablas!E9,_xlfn.CONCAT(" ",$E$26),""),IF(URUGUAY!$C$16=Tablas!E9,_xlfn.CONCAT(" ",$E$27),""),IF(URUGUAY!$C$21=Tablas!E9,_xlfn.CONCAT(" ",$E$28),""),IF(URUGUAY!$C$26=Tablas!E9,_xlfn.CONCAT(" ",$E$29),""))</f>
-        <v xml:space="preserve"> Bella Unión Salto Paysandú</v>
+        <v xml:space="preserve"> Bella Unión</v>
       </c>
       <c r="I28" s="67" t="str">
         <f>_xlfn.CONCAT(I9,IF(G28&gt;1,$J$9,$J$8),H28, IF((G27+G28)=4,".", ";"))</f>
-        <v xml:space="preserve"> se mantiene constante en las ciudades de Bella Unión Salto Paysandú;</v>
+        <v xml:space="preserve"> se mantiene constante en la ciudad de  Bella Unión;</v>
       </c>
       <c r="J28" s="77"/>
       <c r="K28" s="77"/>
       <c r="L28" s="77"/>
     </row>
-    <row r="29" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:13" ht="33" x14ac:dyDescent="0.3">
       <c r="C29" s="53"/>
       <c r="D29" s="53"/>
       <c r="E29" s="53" t="s">
@@ -5412,15 +5387,15 @@
       <c r="F29" s="76"/>
       <c r="G29" s="60">
         <f>SUM(URUGUAY!$C$11=Tablas!E10, URUGUAY!$C$16=Tablas!E10,URUGUAY!$C$21=Tablas!E10,URUGUAY!$C$26=Tablas!E10)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H29" s="61" t="str">
         <f>_xlfn.CONCAT(IF(URUGUAY!$C$11=Tablas!E10,_xlfn.CONCAT(" ",$E$26),""),IF(URUGUAY!$C$16=Tablas!E10,_xlfn.CONCAT(" ",$E$27),""),IF(URUGUAY!$C$21=Tablas!E10,_xlfn.CONCAT(" ",$E$28),""),IF(URUGUAY!$C$26=Tablas!E10,_xlfn.CONCAT(" ",$E$29),""))</f>
-        <v xml:space="preserve"> Fray Bentos</v>
+        <v xml:space="preserve"> Paysandú Fray Bentos</v>
       </c>
       <c r="I29" s="67" t="str">
         <f>_xlfn.CONCAT(I10,IF(G29&gt;1,$J$9,$J$8),H29, ".")</f>
-        <v xml:space="preserve"> está en descenso en la ciudad de  Fray Bentos.</v>
+        <v xml:space="preserve"> está en descenso en las ciudades de Paysandú Fray Bentos.</v>
       </c>
       <c r="J29" s="77"/>
       <c r="K29" s="77"/>
@@ -5438,13 +5413,13 @@
       </c>
       <c r="F30" s="54" t="str">
         <f>_xlfn.CONCAT(IF(OR(MAX(NEGRO!C12:C14)&gt;$D$3,SUM(NEGRO!C12:C14)&gt;$E$3),$F$3,IF(OR(MAX(NEGRO!C12:C14)&gt;$D$4,SUM(NEGRO!C12:C14)&gt;$E$4),$F$4,$F$5)),D30,$I$3,SUM(NEGRO!C12:C14),$J$3,MAX(NEGRO!C12:C14),$K$3)</f>
-        <v>En las últimas horas se registraron bajos acumulados de precipitación en la cuenca del Río Negro, donde en las últimas 72 horas se acumularon 0 mm y con un máximo de 0 mm/día.</v>
+        <v>En las últimas horas se registraron bajos acumulados de precipitación en la cuenca del Río Negro, donde en las últimas 72 horas se acumularon 8 mm y con un máximo de 5.6 mm/día.</v>
       </c>
       <c r="G30" s="54"/>
       <c r="H30" s="54"/>
       <c r="I30" s="66" t="str">
         <f>_xlfn.CONCAT($F$8,D30,IF(NEGRO!C11=$E$8,$I$8,IF(NEGRO!C11=$E$9,$I$9,$I$10)),$J$8,E30,". ")</f>
-        <v xml:space="preserve">Actualmente, el nivel del Río Negro se mantiene constante en la ciudad de Mercedes. </v>
+        <v xml:space="preserve">Actualmente, el nivel del Río Negro está en descenso en la ciudad de Mercedes. </v>
       </c>
       <c r="J30" s="55" t="str">
         <f>_xlfn.CONCAT(F13,IF(NEGRO!C19&gt;NEGRO!C7,I13, IF(NEGRO!C19=NEGRO!C7,I14, I15)))</f>
@@ -5456,7 +5431,7 @@
       </c>
       <c r="L30" s="54" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">En las últimas horas se registraron bajos acumulados de precipitación en la cuenca del Río Negro, donde en las últimas 72 horas se acumularon 0 mm y con un máximo de 0 mm/día. Actualmente, el nivel del Río Negro se mantiene constante en la ciudad de Mercedes.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  </v>
+        <v xml:space="preserve">En las últimas horas se registraron bajos acumulados de precipitación en la cuenca del Río Negro, donde en las últimas 72 horas se acumularon 8 mm y con un máximo de 5.6 mm/día. Actualmente, el nivel del Río Negro está en descenso en la ciudad de Mercedes.  Considerando las lluvias pronosticadas y los niveles registrados en las estaciones de monitoreo, existe la posibilidad de nuevos incrementos de nivel en los próximos días.  </v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RESOLVE ERROR IN THE PLACEHOLDER IMAGE
</commit_message>
<xml_diff>
--- a/automatic docx/database_report.xlsx
+++ b/automatic docx/database_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Sala_Situacion_Dinagua\automatic docx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB75B6E-7C29-443D-AEDD-7D6BED9C6473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C105C1E1-80C2-44DD-9233-2B6741B39FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{83108E16-E9D6-4CCB-B5BE-A67101359CD3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{83108E16-E9D6-4CCB-B5BE-A67101359CD3}"/>
   </bookViews>
   <sheets>
     <sheet name="INICIO" sheetId="1" r:id="rId1"/>
@@ -2177,15 +2177,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1BDC812-2A6B-4705-BA4E-EE32396AA752}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="31.85546875" style="19" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" style="19" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="67" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93.5703125" style="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" style="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="19" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="19"/>
@@ -2222,10 +2222,10 @@
       </c>
       <c r="C3" s="42">
         <f ca="1">TODAY()</f>
-        <v>45786</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>45799</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
         <v>69</v>
       </c>
@@ -2234,10 +2234,10 @@
       </c>
       <c r="C4" s="43">
         <f ca="1">$C$3-1</f>
-        <v>45785</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+        <v>45798</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
         <v>70</v>
       </c>
@@ -2246,10 +2246,10 @@
       </c>
       <c r="C5" s="42">
         <f ca="1">$C$3-2</f>
-        <v>45784</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>45797</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="24" t="s">
         <v>71</v>
       </c>
@@ -2258,10 +2258,10 @@
       </c>
       <c r="C6" s="43">
         <f ca="1">$C$3+1</f>
-        <v>45787</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>45800</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
         <v>72</v>
       </c>
@@ -2270,10 +2270,10 @@
       </c>
       <c r="C7" s="44">
         <f ca="1">$C$3+2</f>
-        <v>45788</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+        <v>45801</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="23" t="s">
         <v>73</v>
       </c>
@@ -2282,7 +2282,7 @@
       </c>
       <c r="C8" s="42">
         <f ca="1">$C$3+3</f>
-        <v>45789</v>
+        <v>45802</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2846,8 +2846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D9A6E30-A876-45F0-8067-30FAF0E80436}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView showGridLines="0" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -3260,7 +3260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE02CEB0-09AB-4ABD-86C9-DCBCC2E88044}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A27" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -3737,13 +3737,13 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" style="16" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="48.28515625" style="5" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="5"/>
   </cols>
@@ -3951,7 +3951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2155F922-1445-4239-A643-A9F5E09853DC}">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
@@ -4925,8 +4925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F783B566-6E24-4EBC-9E3F-D2E3A05600BD}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>